<commit_message>
docs: add sprint 2
</commit_message>
<xml_diff>
--- a/docs/1.-plantilla_sprint.xlsx
+++ b/docs/1.-plantilla_sprint.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PROYECTO_SIS325\Torneos-de-Tenis-de-Mesa-basado-en-llaves\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73FE21D-1CF4-414C-A80A-57ED0BE4E5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3B8191-0C35-4961-9EF6-A97716EABB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -224,7 +224,7 @@
     <numFmt numFmtId="164" formatCode="[$-C0A]d\-mmm\-yy"/>
     <numFmt numFmtId="165" formatCode="[$-C0A]d\-mmm"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -272,6 +272,19 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -761,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -889,10 +902,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -915,6 +924,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -936,6 +949,11 @@
     <xf numFmtId="1" fontId="1" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6974,8 +6992,8 @@
   </sheetPr>
   <dimension ref="A1:AP1002"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7146,7 +7164,7 @@
         <v>44874</v>
       </c>
       <c r="J5" s="26" t="e">
-        <f ca="1">IF(AND(I5&lt;DIA.LAB($E$4,$F$4)-1,I5&lt;&gt;0),DIA.LAB(I5,1,Config!$D$14:$D$25),"")</f>
+        <f ca="1">_xlfn.SINGLE(IF(AND(I5&lt;_xlfn.SINGLE(WORKDAY($E$4,$F$4))-1,I5&lt;&gt;0),D6DIA.LAB(I5,1,Config!$D$14:$D$25),""))</f>
         <v>#NAME?</v>
       </c>
       <c r="K5" s="26" t="e">
@@ -7254,11 +7272,11 @@
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
-      <c r="F6" s="63" t="s">
+      <c r="F6" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
       <c r="I6" s="28">
         <f>COUNTIF(I11:I992,"&gt;0")</f>
         <v>21</v>
@@ -7376,11 +7394,11 @@
       </c>
     </row>
     <row r="7" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F7" s="65" t="s">
+      <c r="F7" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="64"/>
-      <c r="H7" s="66"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="64"/>
       <c r="I7" s="31">
         <f>SUM(I9:I992)</f>
         <v>36</v>
@@ -7491,42 +7509,42 @@
       </c>
     </row>
     <row r="8" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="70" t="s">
+      <c r="B8" s="66"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="71"/>
-      <c r="N8" s="71"/>
-      <c r="O8" s="71"/>
-      <c r="P8" s="71"/>
-      <c r="Q8" s="71"/>
-      <c r="R8" s="71"/>
-      <c r="S8" s="71"/>
-      <c r="T8" s="71"/>
-      <c r="U8" s="71"/>
-      <c r="V8" s="71"/>
-      <c r="W8" s="71"/>
-      <c r="X8" s="71"/>
-      <c r="Y8" s="71"/>
-      <c r="Z8" s="71"/>
-      <c r="AA8" s="71"/>
-      <c r="AB8" s="71"/>
-      <c r="AC8" s="71"/>
-      <c r="AD8" s="71"/>
-      <c r="AE8" s="71"/>
-      <c r="AF8" s="72"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="69"/>
+      <c r="N8" s="69"/>
+      <c r="O8" s="69"/>
+      <c r="P8" s="69"/>
+      <c r="Q8" s="69"/>
+      <c r="R8" s="69"/>
+      <c r="S8" s="69"/>
+      <c r="T8" s="69"/>
+      <c r="U8" s="69"/>
+      <c r="V8" s="69"/>
+      <c r="W8" s="69"/>
+      <c r="X8" s="69"/>
+      <c r="Y8" s="69"/>
+      <c r="Z8" s="69"/>
+      <c r="AA8" s="69"/>
+      <c r="AB8" s="69"/>
+      <c r="AC8" s="69"/>
+      <c r="AD8" s="69"/>
+      <c r="AE8" s="69"/>
+      <c r="AF8" s="70"/>
       <c r="AN8" s="30">
         <f>Config!A16</f>
         <v>0</v>
@@ -7547,11 +7565,11 @@
       <c r="B9" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="67" t="s">
+      <c r="C9" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="68"/>
-      <c r="E9" s="76"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="74"/>
       <c r="F9" s="32" t="s">
         <v>33</v>
       </c>
@@ -7561,30 +7579,30 @@
       <c r="H9" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="73"/>
-      <c r="J9" s="74"/>
-      <c r="K9" s="74"/>
-      <c r="L9" s="74"/>
-      <c r="M9" s="74"/>
-      <c r="N9" s="74"/>
-      <c r="O9" s="74"/>
-      <c r="P9" s="74"/>
-      <c r="Q9" s="74"/>
-      <c r="R9" s="74"/>
-      <c r="S9" s="74"/>
-      <c r="T9" s="74"/>
-      <c r="U9" s="74"/>
-      <c r="V9" s="74"/>
-      <c r="W9" s="74"/>
-      <c r="X9" s="74"/>
-      <c r="Y9" s="74"/>
-      <c r="Z9" s="74"/>
-      <c r="AA9" s="74"/>
-      <c r="AB9" s="74"/>
-      <c r="AC9" s="74"/>
-      <c r="AD9" s="74"/>
-      <c r="AE9" s="74"/>
-      <c r="AF9" s="75"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="72"/>
+      <c r="N9" s="72"/>
+      <c r="O9" s="72"/>
+      <c r="P9" s="72"/>
+      <c r="Q9" s="72"/>
+      <c r="R9" s="72"/>
+      <c r="S9" s="72"/>
+      <c r="T9" s="72"/>
+      <c r="U9" s="72"/>
+      <c r="V9" s="72"/>
+      <c r="W9" s="72"/>
+      <c r="X9" s="72"/>
+      <c r="Y9" s="72"/>
+      <c r="Z9" s="72"/>
+      <c r="AA9" s="72"/>
+      <c r="AB9" s="72"/>
+      <c r="AC9" s="72"/>
+      <c r="AD9" s="72"/>
+      <c r="AE9" s="72"/>
+      <c r="AF9" s="73"/>
       <c r="AG9" s="8"/>
       <c r="AN9" s="30">
         <f>Config!A17</f>
@@ -7606,7 +7624,7 @@
       <c r="B10" s="35">
         <v>1</v>
       </c>
-      <c r="C10" s="62" t="s">
+      <c r="C10" s="75" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="50"/>
@@ -7674,7 +7692,7 @@
       <c r="B11" s="37">
         <v>10</v>
       </c>
-      <c r="C11" s="62" t="s">
+      <c r="C11" s="75" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="50"/>
@@ -7742,7 +7760,7 @@
       <c r="B12" s="37">
         <v>20</v>
       </c>
-      <c r="C12" s="62" t="s">
+      <c r="C12" s="75" t="s">
         <v>38</v>
       </c>
       <c r="D12" s="50"/>
@@ -7810,7 +7828,7 @@
       <c r="B13" s="37">
         <v>30</v>
       </c>
-      <c r="C13" s="62" t="s">
+      <c r="C13" s="75" t="s">
         <v>39</v>
       </c>
       <c r="D13" s="50"/>
@@ -7876,7 +7894,7 @@
       <c r="B14" s="37">
         <v>40</v>
       </c>
-      <c r="C14" s="62" t="s">
+      <c r="C14" s="75" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="50"/>
@@ -7942,7 +7960,7 @@
       <c r="B15" s="37">
         <v>50</v>
       </c>
-      <c r="C15" s="62" t="s">
+      <c r="C15" s="75" t="s">
         <v>41</v>
       </c>
       <c r="D15" s="50"/>
@@ -8008,11 +8026,11 @@
       <c r="B16" s="37">
         <v>60</v>
       </c>
-      <c r="C16" s="62" t="s">
+      <c r="C16" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="51"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="88"/>
       <c r="F16" s="34" t="s">
         <v>13</v>
       </c>
@@ -8133,7 +8151,7 @@
       <c r="B18" s="37">
         <v>70</v>
       </c>
-      <c r="C18" s="62" t="s">
+      <c r="C18" s="75" t="s">
         <v>44</v>
       </c>
       <c r="D18" s="50"/>
@@ -8193,7 +8211,7 @@
       <c r="B19" s="37">
         <v>80</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="75" t="s">
         <v>45</v>
       </c>
       <c r="D19" s="50"/>
@@ -8253,7 +8271,7 @@
       <c r="B20" s="37">
         <v>90</v>
       </c>
-      <c r="C20" s="62" t="s">
+      <c r="C20" s="75" t="s">
         <v>46</v>
       </c>
       <c r="D20" s="50"/>
@@ -8313,7 +8331,7 @@
       <c r="B21" s="37">
         <v>100</v>
       </c>
-      <c r="C21" s="62" t="s">
+      <c r="C21" s="75" t="s">
         <v>47</v>
       </c>
       <c r="D21" s="50"/>
@@ -8361,7 +8379,7 @@
       <c r="B22" s="37">
         <v>110</v>
       </c>
-      <c r="C22" s="62" t="s">
+      <c r="C22" s="75" t="s">
         <v>48</v>
       </c>
       <c r="D22" s="50"/>
@@ -8419,7 +8437,7 @@
       <c r="B23" s="37">
         <v>120</v>
       </c>
-      <c r="C23" s="62" t="s">
+      <c r="C23" s="75" t="s">
         <v>49</v>
       </c>
       <c r="D23" s="50"/>
@@ -8465,7 +8483,7 @@
       <c r="B24" s="37">
         <v>130</v>
       </c>
-      <c r="C24" s="62" t="s">
+      <c r="C24" s="75" t="s">
         <v>50</v>
       </c>
       <c r="D24" s="50"/>
@@ -8511,7 +8529,7 @@
       <c r="B25" s="37">
         <v>140</v>
       </c>
-      <c r="C25" s="62" t="s">
+      <c r="C25" s="75" t="s">
         <v>51</v>
       </c>
       <c r="D25" s="50"/>
@@ -8557,7 +8575,7 @@
       <c r="B26" s="37">
         <v>150</v>
       </c>
-      <c r="C26" s="62" t="s">
+      <c r="C26" s="75" t="s">
         <v>46</v>
       </c>
       <c r="D26" s="50"/>
@@ -8603,7 +8621,7 @@
       <c r="B27" s="37">
         <v>160</v>
       </c>
-      <c r="C27" s="62" t="s">
+      <c r="C27" s="75" t="s">
         <v>52</v>
       </c>
       <c r="D27" s="50"/>
@@ -8649,7 +8667,7 @@
       <c r="B28" s="37">
         <v>170</v>
       </c>
-      <c r="C28" s="62" t="s">
+      <c r="C28" s="75" t="s">
         <v>53</v>
       </c>
       <c r="D28" s="50"/>
@@ -8695,7 +8713,7 @@
       <c r="B29" s="37">
         <v>180</v>
       </c>
-      <c r="C29" s="62" t="s">
+      <c r="C29" s="75" t="s">
         <v>54</v>
       </c>
       <c r="D29" s="50"/>
@@ -8761,7 +8779,7 @@
       <c r="B30" s="37">
         <v>190</v>
       </c>
-      <c r="C30" s="62" t="s">
+      <c r="C30" s="75" t="s">
         <v>55</v>
       </c>
       <c r="D30" s="50"/>
@@ -8807,7 +8825,7 @@
       <c r="B31" s="37">
         <v>200</v>
       </c>
-      <c r="C31" s="62" t="s">
+      <c r="C31" s="75" t="s">
         <v>56</v>
       </c>
       <c r="D31" s="50"/>
@@ -8849,7 +8867,7 @@
     <row r="32" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="34"/>
       <c r="B32" s="37"/>
-      <c r="C32" s="62"/>
+      <c r="C32" s="75"/>
       <c r="D32" s="50"/>
       <c r="E32" s="51"/>
       <c r="F32" s="34"/>
@@ -8883,7 +8901,7 @@
     <row r="33" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="34"/>
       <c r="B33" s="37"/>
-      <c r="C33" s="62"/>
+      <c r="C33" s="75"/>
       <c r="D33" s="50"/>
       <c r="E33" s="51"/>
       <c r="F33" s="34"/>
@@ -8917,7 +8935,7 @@
     <row r="34" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="34"/>
       <c r="B34" s="37"/>
-      <c r="C34" s="62"/>
+      <c r="C34" s="75"/>
       <c r="D34" s="50"/>
       <c r="E34" s="51"/>
       <c r="F34" s="34"/>
@@ -8951,7 +8969,7 @@
     <row r="35" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="34"/>
       <c r="B35" s="37"/>
-      <c r="C35" s="62"/>
+      <c r="C35" s="75"/>
       <c r="D35" s="50"/>
       <c r="E35" s="51"/>
       <c r="F35" s="34"/>
@@ -8985,7 +9003,7 @@
     <row r="36" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="34"/>
       <c r="B36" s="37"/>
-      <c r="C36" s="62"/>
+      <c r="C36" s="75"/>
       <c r="D36" s="50"/>
       <c r="E36" s="51"/>
       <c r="F36" s="34"/>
@@ -9019,7 +9037,7 @@
     <row r="37" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="34"/>
       <c r="B37" s="37"/>
-      <c r="C37" s="62"/>
+      <c r="C37" s="75"/>
       <c r="D37" s="50"/>
       <c r="E37" s="51"/>
       <c r="F37" s="34"/>
@@ -9053,7 +9071,7 @@
     <row r="38" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="40"/>
       <c r="B38" s="37"/>
-      <c r="C38" s="62"/>
+      <c r="C38" s="75"/>
       <c r="D38" s="50"/>
       <c r="E38" s="51"/>
       <c r="F38" s="34"/>
@@ -9087,7 +9105,7 @@
     <row r="39" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="40"/>
       <c r="B39" s="37"/>
-      <c r="C39" s="62"/>
+      <c r="C39" s="75"/>
       <c r="D39" s="50"/>
       <c r="E39" s="51"/>
       <c r="F39" s="34"/>
@@ -9121,7 +9139,7 @@
     <row r="40" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="40"/>
       <c r="B40" s="37"/>
-      <c r="C40" s="62"/>
+      <c r="C40" s="75"/>
       <c r="D40" s="50"/>
       <c r="E40" s="51"/>
       <c r="F40" s="34"/>
@@ -9155,7 +9173,7 @@
     <row r="41" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="40"/>
       <c r="B41" s="37"/>
-      <c r="C41" s="62"/>
+      <c r="C41" s="75"/>
       <c r="D41" s="50"/>
       <c r="E41" s="51"/>
       <c r="F41" s="34"/>
@@ -9189,7 +9207,7 @@
     <row r="42" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="34"/>
       <c r="B42" s="37"/>
-      <c r="C42" s="62"/>
+      <c r="C42" s="75"/>
       <c r="D42" s="50"/>
       <c r="E42" s="51"/>
       <c r="F42" s="34"/>
@@ -9223,7 +9241,7 @@
     <row r="43" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="34"/>
       <c r="B43" s="37"/>
-      <c r="C43" s="62"/>
+      <c r="C43" s="75"/>
       <c r="D43" s="50"/>
       <c r="E43" s="51"/>
       <c r="F43" s="34"/>
@@ -9257,7 +9275,7 @@
     <row r="44" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="34"/>
       <c r="B44" s="37"/>
-      <c r="C44" s="62"/>
+      <c r="C44" s="75"/>
       <c r="D44" s="50"/>
       <c r="E44" s="51"/>
       <c r="F44" s="34"/>
@@ -9291,7 +9309,7 @@
     <row r="45" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="34"/>
       <c r="B45" s="37"/>
-      <c r="C45" s="62"/>
+      <c r="C45" s="75"/>
       <c r="D45" s="50"/>
       <c r="E45" s="51"/>
       <c r="F45" s="34"/>
@@ -9325,7 +9343,7 @@
     <row r="46" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="34"/>
       <c r="B46" s="37"/>
-      <c r="C46" s="62"/>
+      <c r="C46" s="75"/>
       <c r="D46" s="50"/>
       <c r="E46" s="51"/>
       <c r="F46" s="34"/>
@@ -9359,7 +9377,7 @@
     <row r="47" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="34"/>
       <c r="B47" s="37"/>
-      <c r="C47" s="62"/>
+      <c r="C47" s="75"/>
       <c r="D47" s="50"/>
       <c r="E47" s="51"/>
       <c r="F47" s="34"/>
@@ -9393,7 +9411,7 @@
     <row r="48" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="34"/>
       <c r="B48" s="37"/>
-      <c r="C48" s="62"/>
+      <c r="C48" s="75"/>
       <c r="D48" s="50"/>
       <c r="E48" s="51"/>
       <c r="F48" s="34"/>
@@ -9427,7 +9445,7 @@
     <row r="49" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="34"/>
       <c r="B49" s="37"/>
-      <c r="C49" s="62"/>
+      <c r="C49" s="75"/>
       <c r="D49" s="50"/>
       <c r="E49" s="51"/>
       <c r="F49" s="34"/>
@@ -9461,7 +9479,7 @@
     <row r="50" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="34"/>
       <c r="B50" s="37"/>
-      <c r="C50" s="62"/>
+      <c r="C50" s="75"/>
       <c r="D50" s="50"/>
       <c r="E50" s="51"/>
       <c r="F50" s="34"/>
@@ -9495,7 +9513,7 @@
     <row r="51" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="34"/>
       <c r="B51" s="37"/>
-      <c r="C51" s="62"/>
+      <c r="C51" s="75"/>
       <c r="D51" s="50"/>
       <c r="E51" s="51"/>
       <c r="F51" s="34"/>
@@ -9529,7 +9547,7 @@
     <row r="52" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="34"/>
       <c r="B52" s="37"/>
-      <c r="C52" s="62"/>
+      <c r="C52" s="75"/>
       <c r="D52" s="50"/>
       <c r="E52" s="51"/>
       <c r="F52" s="34"/>
@@ -9563,7 +9581,7 @@
     <row r="53" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="34"/>
       <c r="B53" s="37"/>
-      <c r="C53" s="62"/>
+      <c r="C53" s="75"/>
       <c r="D53" s="50"/>
       <c r="E53" s="51"/>
       <c r="F53" s="34"/>
@@ -9597,7 +9615,7 @@
     <row r="54" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="34"/>
       <c r="B54" s="37"/>
-      <c r="C54" s="62"/>
+      <c r="C54" s="75"/>
       <c r="D54" s="50"/>
       <c r="E54" s="51"/>
       <c r="F54" s="34"/>
@@ -9631,7 +9649,7 @@
     <row r="55" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="34"/>
       <c r="B55" s="37"/>
-      <c r="C55" s="62"/>
+      <c r="C55" s="75"/>
       <c r="D55" s="50"/>
       <c r="E55" s="51"/>
       <c r="F55" s="34"/>
@@ -9665,7 +9683,7 @@
     <row r="56" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="34"/>
       <c r="B56" s="37"/>
-      <c r="C56" s="62"/>
+      <c r="C56" s="75"/>
       <c r="D56" s="50"/>
       <c r="E56" s="51"/>
       <c r="F56" s="34"/>
@@ -9699,7 +9717,7 @@
     <row r="57" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="34"/>
       <c r="B57" s="37"/>
-      <c r="C57" s="62"/>
+      <c r="C57" s="75"/>
       <c r="D57" s="50"/>
       <c r="E57" s="51"/>
       <c r="F57" s="34"/>
@@ -9733,7 +9751,7 @@
     <row r="58" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="34"/>
       <c r="B58" s="34"/>
-      <c r="C58" s="61"/>
+      <c r="C58" s="76"/>
       <c r="D58" s="50"/>
       <c r="E58" s="51"/>
       <c r="F58" s="34"/>
@@ -9767,7 +9785,7 @@
     <row r="59" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="34"/>
       <c r="B59" s="34"/>
-      <c r="C59" s="61"/>
+      <c r="C59" s="76"/>
       <c r="D59" s="50"/>
       <c r="E59" s="51"/>
       <c r="F59" s="34"/>
@@ -9801,7 +9819,7 @@
     <row r="60" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="34"/>
       <c r="B60" s="34"/>
-      <c r="C60" s="61"/>
+      <c r="C60" s="76"/>
       <c r="D60" s="50"/>
       <c r="E60" s="51"/>
       <c r="F60" s="34"/>
@@ -9835,7 +9853,7 @@
     <row r="61" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="34"/>
       <c r="B61" s="34"/>
-      <c r="C61" s="61"/>
+      <c r="C61" s="76"/>
       <c r="D61" s="50"/>
       <c r="E61" s="51"/>
       <c r="F61" s="34"/>
@@ -9869,7 +9887,7 @@
     <row r="62" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="34"/>
       <c r="B62" s="34"/>
-      <c r="C62" s="61"/>
+      <c r="C62" s="76"/>
       <c r="D62" s="50"/>
       <c r="E62" s="51"/>
       <c r="F62" s="34"/>
@@ -9903,7 +9921,7 @@
     <row r="63" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="34"/>
       <c r="B63" s="34"/>
-      <c r="C63" s="61"/>
+      <c r="C63" s="76"/>
       <c r="D63" s="50"/>
       <c r="E63" s="51"/>
       <c r="F63" s="34"/>
@@ -9937,7 +9955,7 @@
     <row r="64" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="34"/>
       <c r="B64" s="34"/>
-      <c r="C64" s="61"/>
+      <c r="C64" s="76"/>
       <c r="D64" s="50"/>
       <c r="E64" s="51"/>
       <c r="F64" s="34"/>
@@ -9971,7 +9989,7 @@
     <row r="65" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="34"/>
       <c r="B65" s="34"/>
-      <c r="C65" s="61"/>
+      <c r="C65" s="76"/>
       <c r="D65" s="50"/>
       <c r="E65" s="51"/>
       <c r="F65" s="34"/>
@@ -10005,7 +10023,7 @@
     <row r="66" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="34"/>
       <c r="B66" s="34"/>
-      <c r="C66" s="61"/>
+      <c r="C66" s="76"/>
       <c r="D66" s="50"/>
       <c r="E66" s="51"/>
       <c r="F66" s="34"/>
@@ -10039,7 +10057,7 @@
     <row r="67" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="34"/>
       <c r="B67" s="34"/>
-      <c r="C67" s="61"/>
+      <c r="C67" s="76"/>
       <c r="D67" s="50"/>
       <c r="E67" s="51"/>
       <c r="F67" s="34"/>
@@ -10073,7 +10091,7 @@
     <row r="68" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="34"/>
       <c r="B68" s="34"/>
-      <c r="C68" s="61"/>
+      <c r="C68" s="76"/>
       <c r="D68" s="50"/>
       <c r="E68" s="51"/>
       <c r="F68" s="34"/>
@@ -10107,7 +10125,7 @@
     <row r="69" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="34"/>
       <c r="B69" s="34"/>
-      <c r="C69" s="61"/>
+      <c r="C69" s="76"/>
       <c r="D69" s="50"/>
       <c r="E69" s="51"/>
       <c r="F69" s="34"/>
@@ -10141,7 +10159,7 @@
     <row r="70" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="34"/>
       <c r="B70" s="34"/>
-      <c r="C70" s="61"/>
+      <c r="C70" s="76"/>
       <c r="D70" s="50"/>
       <c r="E70" s="51"/>
       <c r="F70" s="34"/>
@@ -10175,7 +10193,7 @@
     <row r="71" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="34"/>
       <c r="B71" s="34"/>
-      <c r="C71" s="61"/>
+      <c r="C71" s="76"/>
       <c r="D71" s="50"/>
       <c r="E71" s="51"/>
       <c r="F71" s="34"/>
@@ -10209,7 +10227,7 @@
     <row r="72" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="34"/>
       <c r="B72" s="34"/>
-      <c r="C72" s="61"/>
+      <c r="C72" s="76"/>
       <c r="D72" s="50"/>
       <c r="E72" s="51"/>
       <c r="F72" s="34"/>
@@ -10243,7 +10261,7 @@
     <row r="73" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="34"/>
       <c r="B73" s="34"/>
-      <c r="C73" s="61"/>
+      <c r="C73" s="76"/>
       <c r="D73" s="50"/>
       <c r="E73" s="51"/>
       <c r="F73" s="34"/>
@@ -10277,7 +10295,7 @@
     <row r="74" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="34"/>
       <c r="B74" s="34"/>
-      <c r="C74" s="61"/>
+      <c r="C74" s="76"/>
       <c r="D74" s="50"/>
       <c r="E74" s="51"/>
       <c r="F74" s="34"/>
@@ -10311,7 +10329,7 @@
     <row r="75" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="34"/>
       <c r="B75" s="34"/>
-      <c r="C75" s="61"/>
+      <c r="C75" s="76"/>
       <c r="D75" s="50"/>
       <c r="E75" s="51"/>
       <c r="F75" s="34"/>
@@ -10345,7 +10363,7 @@
     <row r="76" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="34"/>
       <c r="B76" s="34"/>
-      <c r="C76" s="61"/>
+      <c r="C76" s="76"/>
       <c r="D76" s="50"/>
       <c r="E76" s="51"/>
       <c r="F76" s="34"/>
@@ -10379,7 +10397,7 @@
     <row r="77" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="34"/>
       <c r="B77" s="34"/>
-      <c r="C77" s="61"/>
+      <c r="C77" s="76"/>
       <c r="D77" s="50"/>
       <c r="E77" s="51"/>
       <c r="F77" s="34"/>
@@ -10413,7 +10431,7 @@
     <row r="78" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="34"/>
       <c r="B78" s="34"/>
-      <c r="C78" s="61"/>
+      <c r="C78" s="76"/>
       <c r="D78" s="50"/>
       <c r="E78" s="51"/>
       <c r="F78" s="34"/>
@@ -10447,7 +10465,7 @@
     <row r="79" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="34"/>
       <c r="B79" s="34"/>
-      <c r="C79" s="61"/>
+      <c r="C79" s="76"/>
       <c r="D79" s="50"/>
       <c r="E79" s="51"/>
       <c r="F79" s="34"/>
@@ -10481,7 +10499,7 @@
     <row r="80" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="34"/>
       <c r="B80" s="34"/>
-      <c r="C80" s="61"/>
+      <c r="C80" s="76"/>
       <c r="D80" s="50"/>
       <c r="E80" s="51"/>
       <c r="F80" s="34"/>
@@ -10515,7 +10533,7 @@
     <row r="81" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="34"/>
       <c r="B81" s="34"/>
-      <c r="C81" s="61"/>
+      <c r="C81" s="76"/>
       <c r="D81" s="50"/>
       <c r="E81" s="51"/>
       <c r="F81" s="34"/>
@@ -10549,7 +10567,7 @@
     <row r="82" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="34"/>
       <c r="B82" s="34"/>
-      <c r="C82" s="61"/>
+      <c r="C82" s="76"/>
       <c r="D82" s="50"/>
       <c r="E82" s="51"/>
       <c r="F82" s="34"/>
@@ -10583,7 +10601,7 @@
     <row r="83" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="34"/>
       <c r="B83" s="34"/>
-      <c r="C83" s="61"/>
+      <c r="C83" s="76"/>
       <c r="D83" s="50"/>
       <c r="E83" s="51"/>
       <c r="F83" s="34"/>
@@ -10617,7 +10635,7 @@
     <row r="84" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="34"/>
       <c r="B84" s="34"/>
-      <c r="C84" s="61"/>
+      <c r="C84" s="76"/>
       <c r="D84" s="50"/>
       <c r="E84" s="51"/>
       <c r="F84" s="34"/>
@@ -10651,7 +10669,7 @@
     <row r="85" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="34"/>
       <c r="B85" s="34"/>
-      <c r="C85" s="61"/>
+      <c r="C85" s="76"/>
       <c r="D85" s="50"/>
       <c r="E85" s="51"/>
       <c r="F85" s="34"/>
@@ -10685,7 +10703,7 @@
     <row r="86" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="34"/>
       <c r="B86" s="34"/>
-      <c r="C86" s="61"/>
+      <c r="C86" s="76"/>
       <c r="D86" s="50"/>
       <c r="E86" s="51"/>
       <c r="F86" s="34"/>
@@ -10719,7 +10737,7 @@
     <row r="87" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="34"/>
       <c r="B87" s="34"/>
-      <c r="C87" s="61"/>
+      <c r="C87" s="76"/>
       <c r="D87" s="50"/>
       <c r="E87" s="51"/>
       <c r="F87" s="34"/>
@@ -10753,7 +10771,7 @@
     <row r="88" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="34"/>
       <c r="B88" s="34"/>
-      <c r="C88" s="61"/>
+      <c r="C88" s="76"/>
       <c r="D88" s="50"/>
       <c r="E88" s="51"/>
       <c r="F88" s="34"/>
@@ -10787,7 +10805,7 @@
     <row r="89" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="34"/>
       <c r="B89" s="34"/>
-      <c r="C89" s="61"/>
+      <c r="C89" s="76"/>
       <c r="D89" s="50"/>
       <c r="E89" s="51"/>
       <c r="F89" s="34"/>
@@ -10821,7 +10839,7 @@
     <row r="90" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="34"/>
       <c r="B90" s="34"/>
-      <c r="C90" s="61"/>
+      <c r="C90" s="76"/>
       <c r="D90" s="50"/>
       <c r="E90" s="51"/>
       <c r="F90" s="34"/>
@@ -10855,7 +10873,7 @@
     <row r="91" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="34"/>
       <c r="B91" s="34"/>
-      <c r="C91" s="61"/>
+      <c r="C91" s="76"/>
       <c r="D91" s="50"/>
       <c r="E91" s="51"/>
       <c r="F91" s="34"/>
@@ -10889,7 +10907,7 @@
     <row r="92" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="34"/>
       <c r="B92" s="34"/>
-      <c r="C92" s="61"/>
+      <c r="C92" s="76"/>
       <c r="D92" s="50"/>
       <c r="E92" s="51"/>
       <c r="F92" s="34"/>
@@ -10923,7 +10941,7 @@
     <row r="93" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="34"/>
       <c r="B93" s="34"/>
-      <c r="C93" s="61"/>
+      <c r="C93" s="76"/>
       <c r="D93" s="50"/>
       <c r="E93" s="51"/>
       <c r="F93" s="34"/>
@@ -10957,7 +10975,7 @@
     <row r="94" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="34"/>
       <c r="B94" s="34"/>
-      <c r="C94" s="61"/>
+      <c r="C94" s="76"/>
       <c r="D94" s="50"/>
       <c r="E94" s="51"/>
       <c r="F94" s="34"/>
@@ -10991,7 +11009,7 @@
     <row r="95" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="34"/>
       <c r="B95" s="34"/>
-      <c r="C95" s="61"/>
+      <c r="C95" s="76"/>
       <c r="D95" s="50"/>
       <c r="E95" s="51"/>
       <c r="F95" s="34"/>
@@ -11025,7 +11043,7 @@
     <row r="96" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="34"/>
       <c r="B96" s="34"/>
-      <c r="C96" s="61"/>
+      <c r="C96" s="76"/>
       <c r="D96" s="50"/>
       <c r="E96" s="51"/>
       <c r="F96" s="34"/>
@@ -11059,7 +11077,7 @@
     <row r="97" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="34"/>
       <c r="B97" s="34"/>
-      <c r="C97" s="61"/>
+      <c r="C97" s="76"/>
       <c r="D97" s="50"/>
       <c r="E97" s="51"/>
       <c r="F97" s="34"/>
@@ -11093,7 +11111,7 @@
     <row r="98" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="34"/>
       <c r="B98" s="34"/>
-      <c r="C98" s="61"/>
+      <c r="C98" s="76"/>
       <c r="D98" s="50"/>
       <c r="E98" s="51"/>
       <c r="F98" s="34"/>
@@ -11127,7 +11145,7 @@
     <row r="99" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="34"/>
       <c r="B99" s="34"/>
-      <c r="C99" s="61"/>
+      <c r="C99" s="76"/>
       <c r="D99" s="50"/>
       <c r="E99" s="51"/>
       <c r="F99" s="34"/>
@@ -11161,7 +11179,7 @@
     <row r="100" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="34"/>
       <c r="B100" s="34"/>
-      <c r="C100" s="61"/>
+      <c r="C100" s="76"/>
       <c r="D100" s="50"/>
       <c r="E100" s="51"/>
       <c r="F100" s="34"/>
@@ -11195,7 +11213,7 @@
     <row r="101" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="34"/>
       <c r="B101" s="34"/>
-      <c r="C101" s="61"/>
+      <c r="C101" s="76"/>
       <c r="D101" s="50"/>
       <c r="E101" s="51"/>
       <c r="F101" s="34"/>
@@ -11229,7 +11247,7 @@
     <row r="102" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
       <c r="B102" s="34"/>
-      <c r="C102" s="61"/>
+      <c r="C102" s="76"/>
       <c r="D102" s="50"/>
       <c r="E102" s="51"/>
       <c r="F102" s="34"/>
@@ -11263,7 +11281,7 @@
     <row r="103" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="34"/>
       <c r="B103" s="34"/>
-      <c r="C103" s="61"/>
+      <c r="C103" s="76"/>
       <c r="D103" s="50"/>
       <c r="E103" s="51"/>
       <c r="F103" s="34"/>
@@ -11297,7 +11315,7 @@
     <row r="104" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="34"/>
       <c r="B104" s="34"/>
-      <c r="C104" s="61"/>
+      <c r="C104" s="76"/>
       <c r="D104" s="50"/>
       <c r="E104" s="51"/>
       <c r="F104" s="34"/>
@@ -11331,7 +11349,7 @@
     <row r="105" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="34"/>
       <c r="B105" s="34"/>
-      <c r="C105" s="61"/>
+      <c r="C105" s="76"/>
       <c r="D105" s="50"/>
       <c r="E105" s="51"/>
       <c r="F105" s="34"/>
@@ -11365,7 +11383,7 @@
     <row r="106" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="34"/>
       <c r="B106" s="34"/>
-      <c r="C106" s="61"/>
+      <c r="C106" s="76"/>
       <c r="D106" s="50"/>
       <c r="E106" s="51"/>
       <c r="F106" s="34"/>
@@ -11399,7 +11417,7 @@
     <row r="107" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="34"/>
       <c r="B107" s="34"/>
-      <c r="C107" s="61"/>
+      <c r="C107" s="76"/>
       <c r="D107" s="50"/>
       <c r="E107" s="51"/>
       <c r="F107" s="34"/>
@@ -11433,7 +11451,7 @@
     <row r="108" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="34"/>
       <c r="B108" s="34"/>
-      <c r="C108" s="61"/>
+      <c r="C108" s="76"/>
       <c r="D108" s="50"/>
       <c r="E108" s="51"/>
       <c r="F108" s="34"/>
@@ -11467,7 +11485,7 @@
     <row r="109" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="34"/>
       <c r="B109" s="34"/>
-      <c r="C109" s="61"/>
+      <c r="C109" s="76"/>
       <c r="D109" s="50"/>
       <c r="E109" s="51"/>
       <c r="F109" s="34"/>
@@ -11501,7 +11519,7 @@
     <row r="110" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="34"/>
       <c r="B110" s="34"/>
-      <c r="C110" s="61"/>
+      <c r="C110" s="76"/>
       <c r="D110" s="50"/>
       <c r="E110" s="51"/>
       <c r="F110" s="34"/>
@@ -11535,7 +11553,7 @@
     <row r="111" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="34"/>
       <c r="B111" s="34"/>
-      <c r="C111" s="61"/>
+      <c r="C111" s="76"/>
       <c r="D111" s="50"/>
       <c r="E111" s="51"/>
       <c r="F111" s="34"/>
@@ -11569,7 +11587,7 @@
     <row r="112" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="34"/>
       <c r="B112" s="34"/>
-      <c r="C112" s="61"/>
+      <c r="C112" s="76"/>
       <c r="D112" s="50"/>
       <c r="E112" s="51"/>
       <c r="F112" s="34"/>
@@ -11603,7 +11621,7 @@
     <row r="113" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="34"/>
       <c r="B113" s="34"/>
-      <c r="C113" s="61"/>
+      <c r="C113" s="76"/>
       <c r="D113" s="50"/>
       <c r="E113" s="51"/>
       <c r="F113" s="34"/>
@@ -11637,7 +11655,7 @@
     <row r="114" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="34"/>
       <c r="B114" s="34"/>
-      <c r="C114" s="61"/>
+      <c r="C114" s="76"/>
       <c r="D114" s="50"/>
       <c r="E114" s="51"/>
       <c r="F114" s="34"/>
@@ -11671,7 +11689,7 @@
     <row r="115" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="34"/>
       <c r="B115" s="34"/>
-      <c r="C115" s="61"/>
+      <c r="C115" s="76"/>
       <c r="D115" s="50"/>
       <c r="E115" s="51"/>
       <c r="F115" s="34"/>
@@ -11705,7 +11723,7 @@
     <row r="116" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="34"/>
       <c r="B116" s="34"/>
-      <c r="C116" s="61"/>
+      <c r="C116" s="76"/>
       <c r="D116" s="50"/>
       <c r="E116" s="51"/>
       <c r="F116" s="34"/>
@@ -11739,7 +11757,7 @@
     <row r="117" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="34"/>
       <c r="B117" s="34"/>
-      <c r="C117" s="61"/>
+      <c r="C117" s="76"/>
       <c r="D117" s="50"/>
       <c r="E117" s="51"/>
       <c r="F117" s="34"/>
@@ -11773,7 +11791,7 @@
     <row r="118" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="34"/>
       <c r="B118" s="34"/>
-      <c r="C118" s="61"/>
+      <c r="C118" s="76"/>
       <c r="D118" s="50"/>
       <c r="E118" s="51"/>
       <c r="F118" s="34"/>
@@ -11807,7 +11825,7 @@
     <row r="119" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="34"/>
       <c r="B119" s="34"/>
-      <c r="C119" s="61"/>
+      <c r="C119" s="76"/>
       <c r="D119" s="50"/>
       <c r="E119" s="51"/>
       <c r="F119" s="34"/>
@@ -11841,7 +11859,7 @@
     <row r="120" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="34"/>
       <c r="B120" s="34"/>
-      <c r="C120" s="61"/>
+      <c r="C120" s="76"/>
       <c r="D120" s="50"/>
       <c r="E120" s="51"/>
       <c r="F120" s="34"/>
@@ -11875,7 +11893,7 @@
     <row r="121" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="34"/>
       <c r="B121" s="34"/>
-      <c r="C121" s="61"/>
+      <c r="C121" s="76"/>
       <c r="D121" s="50"/>
       <c r="E121" s="51"/>
       <c r="F121" s="34"/>
@@ -11909,7 +11927,7 @@
     <row r="122" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="34"/>
       <c r="B122" s="34"/>
-      <c r="C122" s="61"/>
+      <c r="C122" s="76"/>
       <c r="D122" s="50"/>
       <c r="E122" s="51"/>
       <c r="F122" s="34"/>
@@ -11943,7 +11961,7 @@
     <row r="123" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="34"/>
       <c r="B123" s="34"/>
-      <c r="C123" s="61"/>
+      <c r="C123" s="76"/>
       <c r="D123" s="50"/>
       <c r="E123" s="51"/>
       <c r="F123" s="34"/>
@@ -11977,7 +11995,7 @@
     <row r="124" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="34"/>
       <c r="B124" s="34"/>
-      <c r="C124" s="61"/>
+      <c r="C124" s="76"/>
       <c r="D124" s="50"/>
       <c r="E124" s="51"/>
       <c r="F124" s="34"/>
@@ -12011,7 +12029,7 @@
     <row r="125" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="34"/>
       <c r="B125" s="34"/>
-      <c r="C125" s="61"/>
+      <c r="C125" s="76"/>
       <c r="D125" s="50"/>
       <c r="E125" s="51"/>
       <c r="F125" s="34"/>
@@ -12045,7 +12063,7 @@
     <row r="126" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="34"/>
       <c r="B126" s="34"/>
-      <c r="C126" s="61"/>
+      <c r="C126" s="76"/>
       <c r="D126" s="50"/>
       <c r="E126" s="51"/>
       <c r="F126" s="34"/>
@@ -12079,7 +12097,7 @@
     <row r="127" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="34"/>
       <c r="B127" s="34"/>
-      <c r="C127" s="61"/>
+      <c r="C127" s="76"/>
       <c r="D127" s="50"/>
       <c r="E127" s="51"/>
       <c r="F127" s="34"/>
@@ -12113,7 +12131,7 @@
     <row r="128" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="34"/>
       <c r="B128" s="34"/>
-      <c r="C128" s="61"/>
+      <c r="C128" s="76"/>
       <c r="D128" s="50"/>
       <c r="E128" s="51"/>
       <c r="F128" s="34"/>
@@ -12147,7 +12165,7 @@
     <row r="129" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="34"/>
       <c r="B129" s="34"/>
-      <c r="C129" s="61"/>
+      <c r="C129" s="76"/>
       <c r="D129" s="50"/>
       <c r="E129" s="51"/>
       <c r="F129" s="34"/>
@@ -12181,7 +12199,7 @@
     <row r="130" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="34"/>
       <c r="B130" s="34"/>
-      <c r="C130" s="61"/>
+      <c r="C130" s="76"/>
       <c r="D130" s="50"/>
       <c r="E130" s="51"/>
       <c r="F130" s="34"/>
@@ -12215,7 +12233,7 @@
     <row r="131" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="34"/>
       <c r="B131" s="34"/>
-      <c r="C131" s="61"/>
+      <c r="C131" s="76"/>
       <c r="D131" s="50"/>
       <c r="E131" s="51"/>
       <c r="F131" s="34"/>
@@ -12249,7 +12267,7 @@
     <row r="132" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="34"/>
       <c r="B132" s="34"/>
-      <c r="C132" s="61"/>
+      <c r="C132" s="76"/>
       <c r="D132" s="50"/>
       <c r="E132" s="51"/>
       <c r="F132" s="34"/>
@@ -12283,7 +12301,7 @@
     <row r="133" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="34"/>
       <c r="B133" s="34"/>
-      <c r="C133" s="61"/>
+      <c r="C133" s="76"/>
       <c r="D133" s="50"/>
       <c r="E133" s="51"/>
       <c r="F133" s="34"/>
@@ -12317,7 +12335,7 @@
     <row r="134" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="34"/>
       <c r="B134" s="34"/>
-      <c r="C134" s="61"/>
+      <c r="C134" s="76"/>
       <c r="D134" s="50"/>
       <c r="E134" s="51"/>
       <c r="F134" s="34"/>
@@ -12351,7 +12369,7 @@
     <row r="135" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="34"/>
       <c r="B135" s="34"/>
-      <c r="C135" s="61"/>
+      <c r="C135" s="76"/>
       <c r="D135" s="50"/>
       <c r="E135" s="51"/>
       <c r="F135" s="34"/>
@@ -12385,7 +12403,7 @@
     <row r="136" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="34"/>
       <c r="B136" s="34"/>
-      <c r="C136" s="61"/>
+      <c r="C136" s="76"/>
       <c r="D136" s="50"/>
       <c r="E136" s="51"/>
       <c r="F136" s="34"/>
@@ -12419,7 +12437,7 @@
     <row r="137" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="34"/>
       <c r="B137" s="34"/>
-      <c r="C137" s="61"/>
+      <c r="C137" s="76"/>
       <c r="D137" s="50"/>
       <c r="E137" s="51"/>
       <c r="F137" s="34"/>
@@ -12453,7 +12471,7 @@
     <row r="138" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="34"/>
       <c r="B138" s="34"/>
-      <c r="C138" s="61"/>
+      <c r="C138" s="76"/>
       <c r="D138" s="50"/>
       <c r="E138" s="51"/>
       <c r="F138" s="34"/>
@@ -12487,7 +12505,7 @@
     <row r="139" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="34"/>
       <c r="B139" s="34"/>
-      <c r="C139" s="61"/>
+      <c r="C139" s="76"/>
       <c r="D139" s="50"/>
       <c r="E139" s="51"/>
       <c r="F139" s="34"/>
@@ -12521,7 +12539,7 @@
     <row r="140" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="34"/>
       <c r="B140" s="34"/>
-      <c r="C140" s="61"/>
+      <c r="C140" s="76"/>
       <c r="D140" s="50"/>
       <c r="E140" s="51"/>
       <c r="F140" s="34"/>
@@ -12555,7 +12573,7 @@
     <row r="141" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="34"/>
       <c r="B141" s="34"/>
-      <c r="C141" s="61"/>
+      <c r="C141" s="76"/>
       <c r="D141" s="50"/>
       <c r="E141" s="51"/>
       <c r="F141" s="34"/>
@@ -12589,7 +12607,7 @@
     <row r="142" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="34"/>
       <c r="B142" s="34"/>
-      <c r="C142" s="61"/>
+      <c r="C142" s="76"/>
       <c r="D142" s="50"/>
       <c r="E142" s="51"/>
       <c r="F142" s="34"/>
@@ -12623,7 +12641,7 @@
     <row r="143" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="34"/>
       <c r="B143" s="34"/>
-      <c r="C143" s="61"/>
+      <c r="C143" s="76"/>
       <c r="D143" s="50"/>
       <c r="E143" s="51"/>
       <c r="F143" s="34"/>
@@ -12657,7 +12675,7 @@
     <row r="144" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="34"/>
       <c r="B144" s="34"/>
-      <c r="C144" s="61"/>
+      <c r="C144" s="76"/>
       <c r="D144" s="50"/>
       <c r="E144" s="51"/>
       <c r="F144" s="34"/>
@@ -12691,7 +12709,7 @@
     <row r="145" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="34"/>
       <c r="B145" s="34"/>
-      <c r="C145" s="61"/>
+      <c r="C145" s="76"/>
       <c r="D145" s="50"/>
       <c r="E145" s="51"/>
       <c r="F145" s="34"/>
@@ -12725,7 +12743,7 @@
     <row r="146" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="34"/>
       <c r="B146" s="34"/>
-      <c r="C146" s="61"/>
+      <c r="C146" s="76"/>
       <c r="D146" s="50"/>
       <c r="E146" s="51"/>
       <c r="F146" s="34"/>
@@ -12759,7 +12777,7 @@
     <row r="147" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="34"/>
       <c r="B147" s="34"/>
-      <c r="C147" s="61"/>
+      <c r="C147" s="76"/>
       <c r="D147" s="50"/>
       <c r="E147" s="51"/>
       <c r="F147" s="34"/>
@@ -12793,7 +12811,7 @@
     <row r="148" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="34"/>
       <c r="B148" s="34"/>
-      <c r="C148" s="61"/>
+      <c r="C148" s="76"/>
       <c r="D148" s="50"/>
       <c r="E148" s="51"/>
       <c r="F148" s="34"/>
@@ -12827,7 +12845,7 @@
     <row r="149" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="34"/>
       <c r="B149" s="34"/>
-      <c r="C149" s="61"/>
+      <c r="C149" s="76"/>
       <c r="D149" s="50"/>
       <c r="E149" s="51"/>
       <c r="F149" s="34"/>
@@ -12861,7 +12879,7 @@
     <row r="150" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="34"/>
       <c r="B150" s="34"/>
-      <c r="C150" s="61"/>
+      <c r="C150" s="76"/>
       <c r="D150" s="50"/>
       <c r="E150" s="51"/>
       <c r="F150" s="34"/>
@@ -12895,7 +12913,7 @@
     <row r="151" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="34"/>
       <c r="B151" s="34"/>
-      <c r="C151" s="61"/>
+      <c r="C151" s="76"/>
       <c r="D151" s="50"/>
       <c r="E151" s="51"/>
       <c r="F151" s="34"/>
@@ -12929,7 +12947,7 @@
     <row r="152" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="34"/>
       <c r="B152" s="34"/>
-      <c r="C152" s="61"/>
+      <c r="C152" s="76"/>
       <c r="D152" s="50"/>
       <c r="E152" s="51"/>
       <c r="F152" s="34"/>
@@ -12963,7 +12981,7 @@
     <row r="153" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="34"/>
       <c r="B153" s="34"/>
-      <c r="C153" s="61"/>
+      <c r="C153" s="76"/>
       <c r="D153" s="50"/>
       <c r="E153" s="51"/>
       <c r="F153" s="34"/>
@@ -12997,7 +13015,7 @@
     <row r="154" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="34"/>
       <c r="B154" s="34"/>
-      <c r="C154" s="61"/>
+      <c r="C154" s="76"/>
       <c r="D154" s="50"/>
       <c r="E154" s="51"/>
       <c r="F154" s="34"/>
@@ -13031,7 +13049,7 @@
     <row r="155" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="34"/>
       <c r="B155" s="34"/>
-      <c r="C155" s="61"/>
+      <c r="C155" s="76"/>
       <c r="D155" s="50"/>
       <c r="E155" s="51"/>
       <c r="F155" s="34"/>
@@ -13065,7 +13083,7 @@
     <row r="156" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="34"/>
       <c r="B156" s="34"/>
-      <c r="C156" s="61"/>
+      <c r="C156" s="76"/>
       <c r="D156" s="50"/>
       <c r="E156" s="51"/>
       <c r="F156" s="34"/>
@@ -13099,7 +13117,7 @@
     <row r="157" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="34"/>
       <c r="B157" s="34"/>
-      <c r="C157" s="61"/>
+      <c r="C157" s="76"/>
       <c r="D157" s="50"/>
       <c r="E157" s="51"/>
       <c r="F157" s="34"/>
@@ -13133,7 +13151,7 @@
     <row r="158" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="34"/>
       <c r="B158" s="34"/>
-      <c r="C158" s="61"/>
+      <c r="C158" s="76"/>
       <c r="D158" s="50"/>
       <c r="E158" s="51"/>
       <c r="F158" s="34"/>
@@ -13167,7 +13185,7 @@
     <row r="159" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="34"/>
       <c r="B159" s="34"/>
-      <c r="C159" s="61"/>
+      <c r="C159" s="76"/>
       <c r="D159" s="50"/>
       <c r="E159" s="51"/>
       <c r="F159" s="34"/>
@@ -13201,7 +13219,7 @@
     <row r="160" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="34"/>
       <c r="B160" s="34"/>
-      <c r="C160" s="61"/>
+      <c r="C160" s="76"/>
       <c r="D160" s="50"/>
       <c r="E160" s="51"/>
       <c r="F160" s="34"/>
@@ -13235,7 +13253,7 @@
     <row r="161" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="34"/>
       <c r="B161" s="34"/>
-      <c r="C161" s="61"/>
+      <c r="C161" s="76"/>
       <c r="D161" s="50"/>
       <c r="E161" s="51"/>
       <c r="F161" s="34"/>
@@ -13269,7 +13287,7 @@
     <row r="162" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="34"/>
       <c r="B162" s="34"/>
-      <c r="C162" s="61"/>
+      <c r="C162" s="76"/>
       <c r="D162" s="50"/>
       <c r="E162" s="51"/>
       <c r="F162" s="34"/>
@@ -13303,7 +13321,7 @@
     <row r="163" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="34"/>
       <c r="B163" s="34"/>
-      <c r="C163" s="61"/>
+      <c r="C163" s="76"/>
       <c r="D163" s="50"/>
       <c r="E163" s="51"/>
       <c r="F163" s="34"/>
@@ -13337,7 +13355,7 @@
     <row r="164" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="34"/>
       <c r="B164" s="34"/>
-      <c r="C164" s="61"/>
+      <c r="C164" s="76"/>
       <c r="D164" s="50"/>
       <c r="E164" s="51"/>
       <c r="F164" s="34"/>
@@ -13371,7 +13389,7 @@
     <row r="165" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="34"/>
       <c r="B165" s="34"/>
-      <c r="C165" s="61"/>
+      <c r="C165" s="76"/>
       <c r="D165" s="50"/>
       <c r="E165" s="51"/>
       <c r="F165" s="34"/>
@@ -13405,7 +13423,7 @@
     <row r="166" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="34"/>
       <c r="B166" s="34"/>
-      <c r="C166" s="61"/>
+      <c r="C166" s="76"/>
       <c r="D166" s="50"/>
       <c r="E166" s="51"/>
       <c r="F166" s="34"/>
@@ -13439,7 +13457,7 @@
     <row r="167" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="34"/>
       <c r="B167" s="34"/>
-      <c r="C167" s="61"/>
+      <c r="C167" s="76"/>
       <c r="D167" s="50"/>
       <c r="E167" s="51"/>
       <c r="F167" s="34"/>
@@ -13473,7 +13491,7 @@
     <row r="168" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="34"/>
       <c r="B168" s="34"/>
-      <c r="C168" s="61"/>
+      <c r="C168" s="76"/>
       <c r="D168" s="50"/>
       <c r="E168" s="51"/>
       <c r="F168" s="34"/>
@@ -13507,7 +13525,7 @@
     <row r="169" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="34"/>
       <c r="B169" s="34"/>
-      <c r="C169" s="61"/>
+      <c r="C169" s="76"/>
       <c r="D169" s="50"/>
       <c r="E169" s="51"/>
       <c r="F169" s="34"/>
@@ -13541,7 +13559,7 @@
     <row r="170" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="34"/>
       <c r="B170" s="34"/>
-      <c r="C170" s="61"/>
+      <c r="C170" s="76"/>
       <c r="D170" s="50"/>
       <c r="E170" s="51"/>
       <c r="F170" s="34"/>
@@ -13575,7 +13593,7 @@
     <row r="171" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="34"/>
       <c r="B171" s="34"/>
-      <c r="C171" s="61"/>
+      <c r="C171" s="76"/>
       <c r="D171" s="50"/>
       <c r="E171" s="51"/>
       <c r="F171" s="34"/>
@@ -13609,7 +13627,7 @@
     <row r="172" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="34"/>
       <c r="B172" s="34"/>
-      <c r="C172" s="61"/>
+      <c r="C172" s="76"/>
       <c r="D172" s="50"/>
       <c r="E172" s="51"/>
       <c r="F172" s="34"/>
@@ -13643,7 +13661,7 @@
     <row r="173" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="34"/>
       <c r="B173" s="34"/>
-      <c r="C173" s="61"/>
+      <c r="C173" s="76"/>
       <c r="D173" s="50"/>
       <c r="E173" s="51"/>
       <c r="F173" s="34"/>
@@ -13677,7 +13695,7 @@
     <row r="174" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="34"/>
       <c r="B174" s="34"/>
-      <c r="C174" s="61"/>
+      <c r="C174" s="76"/>
       <c r="D174" s="50"/>
       <c r="E174" s="51"/>
       <c r="F174" s="34"/>
@@ -13711,7 +13729,7 @@
     <row r="175" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="34"/>
       <c r="B175" s="34"/>
-      <c r="C175" s="61"/>
+      <c r="C175" s="76"/>
       <c r="D175" s="50"/>
       <c r="E175" s="51"/>
       <c r="F175" s="34"/>
@@ -13745,7 +13763,7 @@
     <row r="176" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="34"/>
       <c r="B176" s="34"/>
-      <c r="C176" s="61"/>
+      <c r="C176" s="76"/>
       <c r="D176" s="50"/>
       <c r="E176" s="51"/>
       <c r="F176" s="34"/>
@@ -13779,7 +13797,7 @@
     <row r="177" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="34"/>
       <c r="B177" s="34"/>
-      <c r="C177" s="61"/>
+      <c r="C177" s="76"/>
       <c r="D177" s="50"/>
       <c r="E177" s="51"/>
       <c r="F177" s="34"/>
@@ -13813,7 +13831,7 @@
     <row r="178" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="34"/>
       <c r="B178" s="34"/>
-      <c r="C178" s="61"/>
+      <c r="C178" s="76"/>
       <c r="D178" s="50"/>
       <c r="E178" s="51"/>
       <c r="F178" s="34"/>
@@ -13847,7 +13865,7 @@
     <row r="179" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="34"/>
       <c r="B179" s="34"/>
-      <c r="C179" s="61"/>
+      <c r="C179" s="76"/>
       <c r="D179" s="50"/>
       <c r="E179" s="51"/>
       <c r="F179" s="34"/>
@@ -13881,7 +13899,7 @@
     <row r="180" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="34"/>
       <c r="B180" s="34"/>
-      <c r="C180" s="61"/>
+      <c r="C180" s="76"/>
       <c r="D180" s="50"/>
       <c r="E180" s="51"/>
       <c r="F180" s="34"/>
@@ -13915,7 +13933,7 @@
     <row r="181" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="34"/>
       <c r="B181" s="34"/>
-      <c r="C181" s="61"/>
+      <c r="C181" s="76"/>
       <c r="D181" s="50"/>
       <c r="E181" s="51"/>
       <c r="F181" s="34"/>
@@ -13949,7 +13967,7 @@
     <row r="182" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="34"/>
       <c r="B182" s="34"/>
-      <c r="C182" s="61"/>
+      <c r="C182" s="76"/>
       <c r="D182" s="50"/>
       <c r="E182" s="51"/>
       <c r="F182" s="34"/>
@@ -13983,7 +14001,7 @@
     <row r="183" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="34"/>
       <c r="B183" s="34"/>
-      <c r="C183" s="61"/>
+      <c r="C183" s="76"/>
       <c r="D183" s="50"/>
       <c r="E183" s="51"/>
       <c r="F183" s="34"/>
@@ -14017,7 +14035,7 @@
     <row r="184" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="34"/>
       <c r="B184" s="34"/>
-      <c r="C184" s="61"/>
+      <c r="C184" s="76"/>
       <c r="D184" s="50"/>
       <c r="E184" s="51"/>
       <c r="F184" s="34"/>
@@ -14051,7 +14069,7 @@
     <row r="185" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="34"/>
       <c r="B185" s="34"/>
-      <c r="C185" s="61"/>
+      <c r="C185" s="76"/>
       <c r="D185" s="50"/>
       <c r="E185" s="51"/>
       <c r="F185" s="34"/>
@@ -14085,7 +14103,7 @@
     <row r="186" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="34"/>
       <c r="B186" s="34"/>
-      <c r="C186" s="61"/>
+      <c r="C186" s="76"/>
       <c r="D186" s="50"/>
       <c r="E186" s="51"/>
       <c r="F186" s="34"/>
@@ -14119,7 +14137,7 @@
     <row r="187" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="34"/>
       <c r="B187" s="34"/>
-      <c r="C187" s="61"/>
+      <c r="C187" s="76"/>
       <c r="D187" s="50"/>
       <c r="E187" s="51"/>
       <c r="F187" s="34"/>
@@ -14153,7 +14171,7 @@
     <row r="188" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="34"/>
       <c r="B188" s="34"/>
-      <c r="C188" s="61"/>
+      <c r="C188" s="76"/>
       <c r="D188" s="50"/>
       <c r="E188" s="51"/>
       <c r="F188" s="34"/>
@@ -14187,7 +14205,7 @@
     <row r="189" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="34"/>
       <c r="B189" s="34"/>
-      <c r="C189" s="61"/>
+      <c r="C189" s="76"/>
       <c r="D189" s="50"/>
       <c r="E189" s="51"/>
       <c r="F189" s="34"/>
@@ -14221,7 +14239,7 @@
     <row r="190" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="34"/>
       <c r="B190" s="34"/>
-      <c r="C190" s="61"/>
+      <c r="C190" s="76"/>
       <c r="D190" s="50"/>
       <c r="E190" s="51"/>
       <c r="F190" s="34"/>
@@ -14255,7 +14273,7 @@
     <row r="191" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="34"/>
       <c r="B191" s="34"/>
-      <c r="C191" s="61"/>
+      <c r="C191" s="76"/>
       <c r="D191" s="50"/>
       <c r="E191" s="51"/>
       <c r="F191" s="34"/>
@@ -14289,7 +14307,7 @@
     <row r="192" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="34"/>
       <c r="B192" s="34"/>
-      <c r="C192" s="61"/>
+      <c r="C192" s="76"/>
       <c r="D192" s="50"/>
       <c r="E192" s="51"/>
       <c r="F192" s="34"/>
@@ -14323,7 +14341,7 @@
     <row r="193" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="34"/>
       <c r="B193" s="34"/>
-      <c r="C193" s="61"/>
+      <c r="C193" s="76"/>
       <c r="D193" s="50"/>
       <c r="E193" s="51"/>
       <c r="F193" s="34"/>
@@ -14357,7 +14375,7 @@
     <row r="194" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="34"/>
       <c r="B194" s="34"/>
-      <c r="C194" s="61"/>
+      <c r="C194" s="76"/>
       <c r="D194" s="50"/>
       <c r="E194" s="51"/>
       <c r="F194" s="34"/>
@@ -14391,7 +14409,7 @@
     <row r="195" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="34"/>
       <c r="B195" s="34"/>
-      <c r="C195" s="61"/>
+      <c r="C195" s="76"/>
       <c r="D195" s="50"/>
       <c r="E195" s="51"/>
       <c r="F195" s="34"/>
@@ -14425,7 +14443,7 @@
     <row r="196" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="34"/>
       <c r="B196" s="34"/>
-      <c r="C196" s="61"/>
+      <c r="C196" s="76"/>
       <c r="D196" s="50"/>
       <c r="E196" s="51"/>
       <c r="F196" s="34"/>
@@ -14459,7 +14477,7 @@
     <row r="197" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="34"/>
       <c r="B197" s="34"/>
-      <c r="C197" s="61"/>
+      <c r="C197" s="76"/>
       <c r="D197" s="50"/>
       <c r="E197" s="51"/>
       <c r="F197" s="34"/>
@@ -14493,7 +14511,7 @@
     <row r="198" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="34"/>
       <c r="B198" s="34"/>
-      <c r="C198" s="61"/>
+      <c r="C198" s="76"/>
       <c r="D198" s="50"/>
       <c r="E198" s="51"/>
       <c r="F198" s="34"/>
@@ -14527,7 +14545,7 @@
     <row r="199" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="34"/>
       <c r="B199" s="34"/>
-      <c r="C199" s="61"/>
+      <c r="C199" s="76"/>
       <c r="D199" s="50"/>
       <c r="E199" s="51"/>
       <c r="F199" s="34"/>
@@ -14561,7 +14579,7 @@
     <row r="200" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="34"/>
       <c r="B200" s="34"/>
-      <c r="C200" s="61"/>
+      <c r="C200" s="76"/>
       <c r="D200" s="50"/>
       <c r="E200" s="51"/>
       <c r="F200" s="34"/>
@@ -14595,7 +14613,7 @@
     <row r="201" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="34"/>
       <c r="B201" s="34"/>
-      <c r="C201" s="61"/>
+      <c r="C201" s="76"/>
       <c r="D201" s="50"/>
       <c r="E201" s="51"/>
       <c r="F201" s="34"/>
@@ -14629,7 +14647,7 @@
     <row r="202" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="34"/>
       <c r="B202" s="34"/>
-      <c r="C202" s="61"/>
+      <c r="C202" s="76"/>
       <c r="D202" s="50"/>
       <c r="E202" s="51"/>
       <c r="F202" s="34"/>
@@ -14663,7 +14681,7 @@
     <row r="203" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="34"/>
       <c r="B203" s="34"/>
-      <c r="C203" s="61"/>
+      <c r="C203" s="76"/>
       <c r="D203" s="50"/>
       <c r="E203" s="51"/>
       <c r="F203" s="34"/>
@@ -14697,7 +14715,7 @@
     <row r="204" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="34"/>
       <c r="B204" s="34"/>
-      <c r="C204" s="61"/>
+      <c r="C204" s="76"/>
       <c r="D204" s="50"/>
       <c r="E204" s="51"/>
       <c r="F204" s="34"/>
@@ -14731,7 +14749,7 @@
     <row r="205" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="34"/>
       <c r="B205" s="34"/>
-      <c r="C205" s="61"/>
+      <c r="C205" s="76"/>
       <c r="D205" s="50"/>
       <c r="E205" s="51"/>
       <c r="F205" s="34"/>
@@ -14765,7 +14783,7 @@
     <row r="206" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="34"/>
       <c r="B206" s="34"/>
-      <c r="C206" s="61"/>
+      <c r="C206" s="76"/>
       <c r="D206" s="50"/>
       <c r="E206" s="51"/>
       <c r="F206" s="34"/>
@@ -14799,7 +14817,7 @@
     <row r="207" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="34"/>
       <c r="B207" s="34"/>
-      <c r="C207" s="61"/>
+      <c r="C207" s="76"/>
       <c r="D207" s="50"/>
       <c r="E207" s="51"/>
       <c r="F207" s="34"/>
@@ -14833,7 +14851,7 @@
     <row r="208" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="34"/>
       <c r="B208" s="34"/>
-      <c r="C208" s="61"/>
+      <c r="C208" s="76"/>
       <c r="D208" s="50"/>
       <c r="E208" s="51"/>
       <c r="F208" s="34"/>
@@ -14867,7 +14885,7 @@
     <row r="209" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="34"/>
       <c r="B209" s="34"/>
-      <c r="C209" s="61"/>
+      <c r="C209" s="76"/>
       <c r="D209" s="50"/>
       <c r="E209" s="51"/>
       <c r="F209" s="34"/>
@@ -14901,7 +14919,7 @@
     <row r="210" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="34"/>
       <c r="B210" s="34"/>
-      <c r="C210" s="61"/>
+      <c r="C210" s="76"/>
       <c r="D210" s="50"/>
       <c r="E210" s="51"/>
       <c r="F210" s="34"/>
@@ -14935,7 +14953,7 @@
     <row r="211" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="34"/>
       <c r="B211" s="34"/>
-      <c r="C211" s="61"/>
+      <c r="C211" s="76"/>
       <c r="D211" s="50"/>
       <c r="E211" s="51"/>
       <c r="F211" s="34"/>
@@ -14969,7 +14987,7 @@
     <row r="212" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="34"/>
       <c r="B212" s="34"/>
-      <c r="C212" s="61"/>
+      <c r="C212" s="76"/>
       <c r="D212" s="50"/>
       <c r="E212" s="51"/>
       <c r="F212" s="34"/>
@@ -15003,7 +15021,7 @@
     <row r="213" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="34"/>
       <c r="B213" s="34"/>
-      <c r="C213" s="61"/>
+      <c r="C213" s="76"/>
       <c r="D213" s="50"/>
       <c r="E213" s="51"/>
       <c r="F213" s="34"/>
@@ -15037,7 +15055,7 @@
     <row r="214" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="34"/>
       <c r="B214" s="34"/>
-      <c r="C214" s="61"/>
+      <c r="C214" s="76"/>
       <c r="D214" s="50"/>
       <c r="E214" s="51"/>
       <c r="F214" s="34"/>
@@ -15071,7 +15089,7 @@
     <row r="215" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="34"/>
       <c r="B215" s="34"/>
-      <c r="C215" s="61"/>
+      <c r="C215" s="76"/>
       <c r="D215" s="50"/>
       <c r="E215" s="51"/>
       <c r="F215" s="34"/>
@@ -15105,7 +15123,7 @@
     <row r="216" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="34"/>
       <c r="B216" s="34"/>
-      <c r="C216" s="61"/>
+      <c r="C216" s="76"/>
       <c r="D216" s="50"/>
       <c r="E216" s="51"/>
       <c r="F216" s="34"/>
@@ -15139,7 +15157,7 @@
     <row r="217" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="34"/>
       <c r="B217" s="34"/>
-      <c r="C217" s="61"/>
+      <c r="C217" s="76"/>
       <c r="D217" s="50"/>
       <c r="E217" s="51"/>
       <c r="F217" s="34"/>
@@ -15173,7 +15191,7 @@
     <row r="218" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="34"/>
       <c r="B218" s="34"/>
-      <c r="C218" s="61"/>
+      <c r="C218" s="76"/>
       <c r="D218" s="50"/>
       <c r="E218" s="51"/>
       <c r="F218" s="34"/>
@@ -15207,7 +15225,7 @@
     <row r="219" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="34"/>
       <c r="B219" s="34"/>
-      <c r="C219" s="61"/>
+      <c r="C219" s="76"/>
       <c r="D219" s="50"/>
       <c r="E219" s="51"/>
       <c r="F219" s="34"/>
@@ -15241,7 +15259,7 @@
     <row r="220" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="34"/>
       <c r="B220" s="34"/>
-      <c r="C220" s="61"/>
+      <c r="C220" s="76"/>
       <c r="D220" s="50"/>
       <c r="E220" s="51"/>
       <c r="F220" s="34"/>
@@ -15275,7 +15293,7 @@
     <row r="221" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="34"/>
       <c r="B221" s="34"/>
-      <c r="C221" s="61"/>
+      <c r="C221" s="76"/>
       <c r="D221" s="50"/>
       <c r="E221" s="51"/>
       <c r="F221" s="34"/>
@@ -15309,7 +15327,7 @@
     <row r="222" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="34"/>
       <c r="B222" s="34"/>
-      <c r="C222" s="61"/>
+      <c r="C222" s="76"/>
       <c r="D222" s="50"/>
       <c r="E222" s="51"/>
       <c r="F222" s="34"/>
@@ -15343,7 +15361,7 @@
     <row r="223" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="34"/>
       <c r="B223" s="34"/>
-      <c r="C223" s="61"/>
+      <c r="C223" s="76"/>
       <c r="D223" s="50"/>
       <c r="E223" s="51"/>
       <c r="F223" s="34"/>
@@ -15377,7 +15395,7 @@
     <row r="224" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="34"/>
       <c r="B224" s="34"/>
-      <c r="C224" s="61"/>
+      <c r="C224" s="76"/>
       <c r="D224" s="50"/>
       <c r="E224" s="51"/>
       <c r="F224" s="34"/>
@@ -15411,7 +15429,7 @@
     <row r="225" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="34"/>
       <c r="B225" s="34"/>
-      <c r="C225" s="61"/>
+      <c r="C225" s="76"/>
       <c r="D225" s="50"/>
       <c r="E225" s="51"/>
       <c r="F225" s="34"/>
@@ -15445,7 +15463,7 @@
     <row r="226" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="34"/>
       <c r="B226" s="34"/>
-      <c r="C226" s="61"/>
+      <c r="C226" s="76"/>
       <c r="D226" s="50"/>
       <c r="E226" s="51"/>
       <c r="F226" s="34"/>
@@ -15479,7 +15497,7 @@
     <row r="227" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="34"/>
       <c r="B227" s="34"/>
-      <c r="C227" s="61"/>
+      <c r="C227" s="76"/>
       <c r="D227" s="50"/>
       <c r="E227" s="51"/>
       <c r="F227" s="34"/>
@@ -15513,7 +15531,7 @@
     <row r="228" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="34"/>
       <c r="B228" s="34"/>
-      <c r="C228" s="61"/>
+      <c r="C228" s="76"/>
       <c r="D228" s="50"/>
       <c r="E228" s="51"/>
       <c r="F228" s="34"/>
@@ -15547,7 +15565,7 @@
     <row r="229" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="34"/>
       <c r="B229" s="34"/>
-      <c r="C229" s="61"/>
+      <c r="C229" s="76"/>
       <c r="D229" s="50"/>
       <c r="E229" s="51"/>
       <c r="F229" s="34"/>
@@ -15581,7 +15599,7 @@
     <row r="230" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="34"/>
       <c r="B230" s="34"/>
-      <c r="C230" s="61"/>
+      <c r="C230" s="76"/>
       <c r="D230" s="50"/>
       <c r="E230" s="51"/>
       <c r="F230" s="34"/>
@@ -15615,7 +15633,7 @@
     <row r="231" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="34"/>
       <c r="B231" s="34"/>
-      <c r="C231" s="61"/>
+      <c r="C231" s="76"/>
       <c r="D231" s="50"/>
       <c r="E231" s="51"/>
       <c r="F231" s="34"/>
@@ -17504,150 +17522,64 @@
   </sheetData>
   <autoFilter ref="A9:H24" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="226">
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="I8:AF9"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="C77:E77"/>
-    <mergeCell ref="C78:E78"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="C81:E81"/>
-    <mergeCell ref="C82:E82"/>
-    <mergeCell ref="C83:E83"/>
-    <mergeCell ref="C84:E84"/>
-    <mergeCell ref="C85:E85"/>
-    <mergeCell ref="C86:E86"/>
-    <mergeCell ref="C87:E87"/>
-    <mergeCell ref="C88:E88"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C90:E90"/>
-    <mergeCell ref="C91:E91"/>
-    <mergeCell ref="C92:E92"/>
-    <mergeCell ref="C93:E93"/>
-    <mergeCell ref="C94:E94"/>
-    <mergeCell ref="C95:E95"/>
-    <mergeCell ref="C96:E96"/>
-    <mergeCell ref="C97:E97"/>
-    <mergeCell ref="C98:E98"/>
-    <mergeCell ref="C99:E99"/>
-    <mergeCell ref="C100:E100"/>
-    <mergeCell ref="C101:E101"/>
-    <mergeCell ref="C102:E102"/>
-    <mergeCell ref="C103:E103"/>
-    <mergeCell ref="C104:E104"/>
-    <mergeCell ref="C105:E105"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C107:E107"/>
-    <mergeCell ref="C108:E108"/>
-    <mergeCell ref="C109:E109"/>
-    <mergeCell ref="C110:E110"/>
-    <mergeCell ref="C111:E111"/>
-    <mergeCell ref="C112:E112"/>
-    <mergeCell ref="C113:E113"/>
-    <mergeCell ref="C114:E114"/>
-    <mergeCell ref="C115:E115"/>
-    <mergeCell ref="C116:E116"/>
-    <mergeCell ref="C117:E117"/>
-    <mergeCell ref="C118:E118"/>
-    <mergeCell ref="C119:E119"/>
-    <mergeCell ref="C120:E120"/>
-    <mergeCell ref="C121:E121"/>
-    <mergeCell ref="C122:E122"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C124:E124"/>
-    <mergeCell ref="C125:E125"/>
-    <mergeCell ref="C126:E126"/>
-    <mergeCell ref="C127:E127"/>
-    <mergeCell ref="C128:E128"/>
-    <mergeCell ref="C129:E129"/>
-    <mergeCell ref="C130:E130"/>
-    <mergeCell ref="C131:E131"/>
-    <mergeCell ref="C132:E132"/>
-    <mergeCell ref="C133:E133"/>
-    <mergeCell ref="C134:E134"/>
-    <mergeCell ref="C135:E135"/>
-    <mergeCell ref="C136:E136"/>
-    <mergeCell ref="C137:E137"/>
-    <mergeCell ref="C138:E138"/>
-    <mergeCell ref="C139:E139"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C141:E141"/>
-    <mergeCell ref="C142:E142"/>
-    <mergeCell ref="C143:E143"/>
-    <mergeCell ref="C144:E144"/>
-    <mergeCell ref="C145:E145"/>
-    <mergeCell ref="C146:E146"/>
-    <mergeCell ref="C147:E147"/>
-    <mergeCell ref="C148:E148"/>
-    <mergeCell ref="C149:E149"/>
+    <mergeCell ref="C196:E196"/>
+    <mergeCell ref="C197:E197"/>
+    <mergeCell ref="C198:E198"/>
+    <mergeCell ref="C199:E199"/>
+    <mergeCell ref="C200:E200"/>
+    <mergeCell ref="C201:E201"/>
+    <mergeCell ref="C202:E202"/>
+    <mergeCell ref="C187:E187"/>
+    <mergeCell ref="C188:E188"/>
+    <mergeCell ref="C189:E189"/>
+    <mergeCell ref="C190:E190"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C192:E192"/>
+    <mergeCell ref="C193:E193"/>
+    <mergeCell ref="C194:E194"/>
+    <mergeCell ref="C195:E195"/>
+    <mergeCell ref="C178:E178"/>
+    <mergeCell ref="C179:E179"/>
+    <mergeCell ref="C180:E180"/>
+    <mergeCell ref="C181:E181"/>
+    <mergeCell ref="C182:E182"/>
+    <mergeCell ref="C183:E183"/>
+    <mergeCell ref="C184:E184"/>
+    <mergeCell ref="C185:E185"/>
+    <mergeCell ref="C186:E186"/>
+    <mergeCell ref="C169:E169"/>
+    <mergeCell ref="C170:E170"/>
+    <mergeCell ref="C171:E171"/>
+    <mergeCell ref="C172:E172"/>
+    <mergeCell ref="C173:E173"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C175:E175"/>
+    <mergeCell ref="C176:E176"/>
+    <mergeCell ref="C177:E177"/>
+    <mergeCell ref="C224:E224"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C226:E226"/>
+    <mergeCell ref="C227:E227"/>
+    <mergeCell ref="C228:E228"/>
+    <mergeCell ref="C229:E229"/>
+    <mergeCell ref="C230:E230"/>
+    <mergeCell ref="C231:E231"/>
+    <mergeCell ref="C217:E217"/>
+    <mergeCell ref="C218:E218"/>
+    <mergeCell ref="C219:E219"/>
+    <mergeCell ref="C220:E220"/>
+    <mergeCell ref="C221:E221"/>
+    <mergeCell ref="C222:E222"/>
+    <mergeCell ref="C223:E223"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="C215:E215"/>
+    <mergeCell ref="C216:E216"/>
     <mergeCell ref="C150:E150"/>
     <mergeCell ref="C151:E151"/>
     <mergeCell ref="C152:E152"/>
@@ -17672,64 +17604,150 @@
     <mergeCell ref="C166:E166"/>
     <mergeCell ref="C167:E167"/>
     <mergeCell ref="C168:E168"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="C215:E215"/>
-    <mergeCell ref="C216:E216"/>
-    <mergeCell ref="C224:E224"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C226:E226"/>
-    <mergeCell ref="C227:E227"/>
-    <mergeCell ref="C228:E228"/>
-    <mergeCell ref="C229:E229"/>
-    <mergeCell ref="C230:E230"/>
-    <mergeCell ref="C231:E231"/>
-    <mergeCell ref="C217:E217"/>
-    <mergeCell ref="C218:E218"/>
-    <mergeCell ref="C219:E219"/>
-    <mergeCell ref="C220:E220"/>
-    <mergeCell ref="C221:E221"/>
-    <mergeCell ref="C222:E222"/>
-    <mergeCell ref="C223:E223"/>
-    <mergeCell ref="C169:E169"/>
-    <mergeCell ref="C170:E170"/>
-    <mergeCell ref="C171:E171"/>
-    <mergeCell ref="C172:E172"/>
-    <mergeCell ref="C173:E173"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C175:E175"/>
-    <mergeCell ref="C176:E176"/>
-    <mergeCell ref="C177:E177"/>
-    <mergeCell ref="C178:E178"/>
-    <mergeCell ref="C179:E179"/>
-    <mergeCell ref="C180:E180"/>
-    <mergeCell ref="C181:E181"/>
-    <mergeCell ref="C182:E182"/>
-    <mergeCell ref="C183:E183"/>
-    <mergeCell ref="C184:E184"/>
-    <mergeCell ref="C185:E185"/>
-    <mergeCell ref="C186:E186"/>
-    <mergeCell ref="C196:E196"/>
-    <mergeCell ref="C197:E197"/>
-    <mergeCell ref="C198:E198"/>
-    <mergeCell ref="C199:E199"/>
-    <mergeCell ref="C200:E200"/>
-    <mergeCell ref="C201:E201"/>
-    <mergeCell ref="C202:E202"/>
-    <mergeCell ref="C187:E187"/>
-    <mergeCell ref="C188:E188"/>
-    <mergeCell ref="C189:E189"/>
-    <mergeCell ref="C190:E190"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="C192:E192"/>
-    <mergeCell ref="C193:E193"/>
-    <mergeCell ref="C194:E194"/>
-    <mergeCell ref="C195:E195"/>
+    <mergeCell ref="C141:E141"/>
+    <mergeCell ref="C142:E142"/>
+    <mergeCell ref="C143:E143"/>
+    <mergeCell ref="C144:E144"/>
+    <mergeCell ref="C145:E145"/>
+    <mergeCell ref="C146:E146"/>
+    <mergeCell ref="C147:E147"/>
+    <mergeCell ref="C148:E148"/>
+    <mergeCell ref="C149:E149"/>
+    <mergeCell ref="C132:E132"/>
+    <mergeCell ref="C133:E133"/>
+    <mergeCell ref="C134:E134"/>
+    <mergeCell ref="C135:E135"/>
+    <mergeCell ref="C136:E136"/>
+    <mergeCell ref="C137:E137"/>
+    <mergeCell ref="C138:E138"/>
+    <mergeCell ref="C139:E139"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C124:E124"/>
+    <mergeCell ref="C125:E125"/>
+    <mergeCell ref="C126:E126"/>
+    <mergeCell ref="C127:E127"/>
+    <mergeCell ref="C128:E128"/>
+    <mergeCell ref="C129:E129"/>
+    <mergeCell ref="C130:E130"/>
+    <mergeCell ref="C131:E131"/>
+    <mergeCell ref="C114:E114"/>
+    <mergeCell ref="C115:E115"/>
+    <mergeCell ref="C116:E116"/>
+    <mergeCell ref="C117:E117"/>
+    <mergeCell ref="C118:E118"/>
+    <mergeCell ref="C119:E119"/>
+    <mergeCell ref="C120:E120"/>
+    <mergeCell ref="C121:E121"/>
+    <mergeCell ref="C122:E122"/>
+    <mergeCell ref="C105:E105"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C107:E107"/>
+    <mergeCell ref="C108:E108"/>
+    <mergeCell ref="C109:E109"/>
+    <mergeCell ref="C110:E110"/>
+    <mergeCell ref="C111:E111"/>
+    <mergeCell ref="C112:E112"/>
+    <mergeCell ref="C113:E113"/>
+    <mergeCell ref="C96:E96"/>
+    <mergeCell ref="C97:E97"/>
+    <mergeCell ref="C98:E98"/>
+    <mergeCell ref="C99:E99"/>
+    <mergeCell ref="C100:E100"/>
+    <mergeCell ref="C101:E101"/>
+    <mergeCell ref="C102:E102"/>
+    <mergeCell ref="C103:E103"/>
+    <mergeCell ref="C104:E104"/>
+    <mergeCell ref="C87:E87"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C90:E90"/>
+    <mergeCell ref="C91:E91"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="C93:E93"/>
+    <mergeCell ref="C94:E94"/>
+    <mergeCell ref="C95:E95"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="C81:E81"/>
+    <mergeCell ref="C82:E82"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="C84:E84"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="C86:E86"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C77:E77"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="I8:AF9"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C13:E13"/>
   </mergeCells>
   <conditionalFormatting sqref="G991:G1002">
     <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">

</xml_diff>

<commit_message>
docs: sprint 2 was modified
</commit_message>
<xml_diff>
--- a/docs/1.-plantilla_sprint.xlsx
+++ b/docs/1.-plantilla_sprint.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PROYECTO_SIS325\Torneos-de-Tenis-de-Mesa-basado-en-llaves\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ProyectoSIS325\Torneos-de-Tenis-de-Mesa-basado-en-llaves\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3B8191-0C35-4961-9EF6-A97716EABB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78915738-E5AC-4708-821E-B47485C82BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instrucciones" sheetId="1" r:id="rId1"/>
@@ -902,6 +902,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -924,10 +933,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -949,11 +954,6 @@
     <xf numFmtId="1" fontId="1" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1279,13 +1279,13 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2</c:v>
@@ -2080,13 +2080,13 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2476,7 +2476,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2</c:v>
@@ -6992,8 +6992,8 @@
   </sheetPr>
   <dimension ref="A1:AP1002"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:E16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7272,11 +7272,11 @@
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
-      <c r="F6" s="61" t="s">
+      <c r="F6" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
       <c r="I6" s="28">
         <f>COUNTIF(I11:I992,"&gt;0")</f>
         <v>21</v>
@@ -7394,26 +7394,26 @@
       </c>
     </row>
     <row r="7" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F7" s="63" t="s">
+      <c r="F7" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="62"/>
-      <c r="H7" s="64"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="69"/>
       <c r="I7" s="31">
         <f>SUM(I9:I992)</f>
         <v>36</v>
       </c>
       <c r="J7" s="31">
         <f t="shared" ref="J7:AF7" si="2">SUM(J9:J1003)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K7" s="31">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L7" s="31">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M7" s="31">
         <f t="shared" si="2"/>
@@ -7509,42 +7509,42 @@
       </c>
     </row>
     <row r="8" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="68" t="s">
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
-      <c r="O8" s="69"/>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="69"/>
-      <c r="S8" s="69"/>
-      <c r="T8" s="69"/>
-      <c r="U8" s="69"/>
-      <c r="V8" s="69"/>
-      <c r="W8" s="69"/>
-      <c r="X8" s="69"/>
-      <c r="Y8" s="69"/>
-      <c r="Z8" s="69"/>
-      <c r="AA8" s="69"/>
-      <c r="AB8" s="69"/>
-      <c r="AC8" s="69"/>
-      <c r="AD8" s="69"/>
-      <c r="AE8" s="69"/>
-      <c r="AF8" s="70"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="74"/>
+      <c r="Q8" s="74"/>
+      <c r="R8" s="74"/>
+      <c r="S8" s="74"/>
+      <c r="T8" s="74"/>
+      <c r="U8" s="74"/>
+      <c r="V8" s="74"/>
+      <c r="W8" s="74"/>
+      <c r="X8" s="74"/>
+      <c r="Y8" s="74"/>
+      <c r="Z8" s="74"/>
+      <c r="AA8" s="74"/>
+      <c r="AB8" s="74"/>
+      <c r="AC8" s="74"/>
+      <c r="AD8" s="74"/>
+      <c r="AE8" s="74"/>
+      <c r="AF8" s="75"/>
       <c r="AN8" s="30">
         <f>Config!A16</f>
         <v>0</v>
@@ -7565,11 +7565,11 @@
       <c r="B9" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="65" t="s">
+      <c r="C9" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="66"/>
-      <c r="E9" s="74"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="79"/>
       <c r="F9" s="32" t="s">
         <v>33</v>
       </c>
@@ -7579,30 +7579,30 @@
       <c r="H9" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="71"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="72"/>
-      <c r="N9" s="72"/>
-      <c r="O9" s="72"/>
-      <c r="P9" s="72"/>
-      <c r="Q9" s="72"/>
-      <c r="R9" s="72"/>
-      <c r="S9" s="72"/>
-      <c r="T9" s="72"/>
-      <c r="U9" s="72"/>
-      <c r="V9" s="72"/>
-      <c r="W9" s="72"/>
-      <c r="X9" s="72"/>
-      <c r="Y9" s="72"/>
-      <c r="Z9" s="72"/>
-      <c r="AA9" s="72"/>
-      <c r="AB9" s="72"/>
-      <c r="AC9" s="72"/>
-      <c r="AD9" s="72"/>
-      <c r="AE9" s="72"/>
-      <c r="AF9" s="73"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="77"/>
+      <c r="K9" s="77"/>
+      <c r="L9" s="77"/>
+      <c r="M9" s="77"/>
+      <c r="N9" s="77"/>
+      <c r="O9" s="77"/>
+      <c r="P9" s="77"/>
+      <c r="Q9" s="77"/>
+      <c r="R9" s="77"/>
+      <c r="S9" s="77"/>
+      <c r="T9" s="77"/>
+      <c r="U9" s="77"/>
+      <c r="V9" s="77"/>
+      <c r="W9" s="77"/>
+      <c r="X9" s="77"/>
+      <c r="Y9" s="77"/>
+      <c r="Z9" s="77"/>
+      <c r="AA9" s="77"/>
+      <c r="AB9" s="77"/>
+      <c r="AC9" s="77"/>
+      <c r="AD9" s="77"/>
+      <c r="AE9" s="77"/>
+      <c r="AF9" s="78"/>
       <c r="AG9" s="8"/>
       <c r="AN9" s="30">
         <f>Config!A17</f>
@@ -7624,7 +7624,7 @@
       <c r="B10" s="35">
         <v>1</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="62" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="50"/>
@@ -7692,7 +7692,7 @@
       <c r="B11" s="37">
         <v>10</v>
       </c>
-      <c r="C11" s="75" t="s">
+      <c r="C11" s="62" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="50"/>
@@ -7760,7 +7760,7 @@
       <c r="B12" s="37">
         <v>20</v>
       </c>
-      <c r="C12" s="75" t="s">
+      <c r="C12" s="62" t="s">
         <v>38</v>
       </c>
       <c r="D12" s="50"/>
@@ -7828,7 +7828,7 @@
       <c r="B13" s="37">
         <v>30</v>
       </c>
-      <c r="C13" s="75" t="s">
+      <c r="C13" s="62" t="s">
         <v>39</v>
       </c>
       <c r="D13" s="50"/>
@@ -7894,7 +7894,7 @@
       <c r="B14" s="37">
         <v>40</v>
       </c>
-      <c r="C14" s="75" t="s">
+      <c r="C14" s="62" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="50"/>
@@ -7960,7 +7960,7 @@
       <c r="B15" s="37">
         <v>50</v>
       </c>
-      <c r="C15" s="75" t="s">
+      <c r="C15" s="62" t="s">
         <v>41</v>
       </c>
       <c r="D15" s="50"/>
@@ -8026,11 +8026,11 @@
       <c r="B16" s="37">
         <v>60</v>
       </c>
-      <c r="C16" s="86" t="s">
+      <c r="C16" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="87"/>
-      <c r="E16" s="88"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="65"/>
       <c r="F16" s="34" t="s">
         <v>13</v>
       </c>
@@ -8050,7 +8050,7 @@
         <v>2</v>
       </c>
       <c r="L16" s="36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M16" s="36">
         <v>1</v>
@@ -8112,13 +8112,13 @@
         <v>2</v>
       </c>
       <c r="J17" s="36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K17" s="36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L17" s="36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M17" s="36"/>
       <c r="N17" s="34"/>
@@ -8151,7 +8151,7 @@
       <c r="B18" s="37">
         <v>70</v>
       </c>
-      <c r="C18" s="75" t="s">
+      <c r="C18" s="62" t="s">
         <v>44</v>
       </c>
       <c r="D18" s="50"/>
@@ -8211,7 +8211,7 @@
       <c r="B19" s="37">
         <v>80</v>
       </c>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="62" t="s">
         <v>45</v>
       </c>
       <c r="D19" s="50"/>
@@ -8271,7 +8271,7 @@
       <c r="B20" s="37">
         <v>90</v>
       </c>
-      <c r="C20" s="75" t="s">
+      <c r="C20" s="62" t="s">
         <v>46</v>
       </c>
       <c r="D20" s="50"/>
@@ -8331,7 +8331,7 @@
       <c r="B21" s="37">
         <v>100</v>
       </c>
-      <c r="C21" s="75" t="s">
+      <c r="C21" s="62" t="s">
         <v>47</v>
       </c>
       <c r="D21" s="50"/>
@@ -8374,12 +8374,12 @@
     </row>
     <row r="22" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B22" s="37">
         <v>110</v>
       </c>
-      <c r="C22" s="75" t="s">
+      <c r="C22" s="62" t="s">
         <v>48</v>
       </c>
       <c r="D22" s="50"/>
@@ -8437,7 +8437,7 @@
       <c r="B23" s="37">
         <v>120</v>
       </c>
-      <c r="C23" s="75" t="s">
+      <c r="C23" s="62" t="s">
         <v>49</v>
       </c>
       <c r="D23" s="50"/>
@@ -8483,7 +8483,7 @@
       <c r="B24" s="37">
         <v>130</v>
       </c>
-      <c r="C24" s="75" t="s">
+      <c r="C24" s="62" t="s">
         <v>50</v>
       </c>
       <c r="D24" s="50"/>
@@ -8529,7 +8529,7 @@
       <c r="B25" s="37">
         <v>140</v>
       </c>
-      <c r="C25" s="75" t="s">
+      <c r="C25" s="62" t="s">
         <v>51</v>
       </c>
       <c r="D25" s="50"/>
@@ -8575,7 +8575,7 @@
       <c r="B26" s="37">
         <v>150</v>
       </c>
-      <c r="C26" s="75" t="s">
+      <c r="C26" s="62" t="s">
         <v>46</v>
       </c>
       <c r="D26" s="50"/>
@@ -8621,7 +8621,7 @@
       <c r="B27" s="37">
         <v>160</v>
       </c>
-      <c r="C27" s="75" t="s">
+      <c r="C27" s="62" t="s">
         <v>52</v>
       </c>
       <c r="D27" s="50"/>
@@ -8667,7 +8667,7 @@
       <c r="B28" s="37">
         <v>170</v>
       </c>
-      <c r="C28" s="75" t="s">
+      <c r="C28" s="62" t="s">
         <v>53</v>
       </c>
       <c r="D28" s="50"/>
@@ -8713,7 +8713,7 @@
       <c r="B29" s="37">
         <v>180</v>
       </c>
-      <c r="C29" s="75" t="s">
+      <c r="C29" s="62" t="s">
         <v>54</v>
       </c>
       <c r="D29" s="50"/>
@@ -8779,7 +8779,7 @@
       <c r="B30" s="37">
         <v>190</v>
       </c>
-      <c r="C30" s="75" t="s">
+      <c r="C30" s="62" t="s">
         <v>55</v>
       </c>
       <c r="D30" s="50"/>
@@ -8825,7 +8825,7 @@
       <c r="B31" s="37">
         <v>200</v>
       </c>
-      <c r="C31" s="75" t="s">
+      <c r="C31" s="62" t="s">
         <v>56</v>
       </c>
       <c r="D31" s="50"/>
@@ -8867,7 +8867,7 @@
     <row r="32" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="34"/>
       <c r="B32" s="37"/>
-      <c r="C32" s="75"/>
+      <c r="C32" s="62"/>
       <c r="D32" s="50"/>
       <c r="E32" s="51"/>
       <c r="F32" s="34"/>
@@ -8901,7 +8901,7 @@
     <row r="33" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="34"/>
       <c r="B33" s="37"/>
-      <c r="C33" s="75"/>
+      <c r="C33" s="62"/>
       <c r="D33" s="50"/>
       <c r="E33" s="51"/>
       <c r="F33" s="34"/>
@@ -8935,7 +8935,7 @@
     <row r="34" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="34"/>
       <c r="B34" s="37"/>
-      <c r="C34" s="75"/>
+      <c r="C34" s="62"/>
       <c r="D34" s="50"/>
       <c r="E34" s="51"/>
       <c r="F34" s="34"/>
@@ -8969,7 +8969,7 @@
     <row r="35" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="34"/>
       <c r="B35" s="37"/>
-      <c r="C35" s="75"/>
+      <c r="C35" s="62"/>
       <c r="D35" s="50"/>
       <c r="E35" s="51"/>
       <c r="F35" s="34"/>
@@ -9003,7 +9003,7 @@
     <row r="36" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="34"/>
       <c r="B36" s="37"/>
-      <c r="C36" s="75"/>
+      <c r="C36" s="62"/>
       <c r="D36" s="50"/>
       <c r="E36" s="51"/>
       <c r="F36" s="34"/>
@@ -9037,7 +9037,7 @@
     <row r="37" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="34"/>
       <c r="B37" s="37"/>
-      <c r="C37" s="75"/>
+      <c r="C37" s="62"/>
       <c r="D37" s="50"/>
       <c r="E37" s="51"/>
       <c r="F37" s="34"/>
@@ -9071,7 +9071,7 @@
     <row r="38" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="40"/>
       <c r="B38" s="37"/>
-      <c r="C38" s="75"/>
+      <c r="C38" s="62"/>
       <c r="D38" s="50"/>
       <c r="E38" s="51"/>
       <c r="F38" s="34"/>
@@ -9105,7 +9105,7 @@
     <row r="39" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="40"/>
       <c r="B39" s="37"/>
-      <c r="C39" s="75"/>
+      <c r="C39" s="62"/>
       <c r="D39" s="50"/>
       <c r="E39" s="51"/>
       <c r="F39" s="34"/>
@@ -9139,7 +9139,7 @@
     <row r="40" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="40"/>
       <c r="B40" s="37"/>
-      <c r="C40" s="75"/>
+      <c r="C40" s="62"/>
       <c r="D40" s="50"/>
       <c r="E40" s="51"/>
       <c r="F40" s="34"/>
@@ -9173,7 +9173,7 @@
     <row r="41" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="40"/>
       <c r="B41" s="37"/>
-      <c r="C41" s="75"/>
+      <c r="C41" s="62"/>
       <c r="D41" s="50"/>
       <c r="E41" s="51"/>
       <c r="F41" s="34"/>
@@ -9207,7 +9207,7 @@
     <row r="42" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="34"/>
       <c r="B42" s="37"/>
-      <c r="C42" s="75"/>
+      <c r="C42" s="62"/>
       <c r="D42" s="50"/>
       <c r="E42" s="51"/>
       <c r="F42" s="34"/>
@@ -9241,7 +9241,7 @@
     <row r="43" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="34"/>
       <c r="B43" s="37"/>
-      <c r="C43" s="75"/>
+      <c r="C43" s="62"/>
       <c r="D43" s="50"/>
       <c r="E43" s="51"/>
       <c r="F43" s="34"/>
@@ -9275,7 +9275,7 @@
     <row r="44" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="34"/>
       <c r="B44" s="37"/>
-      <c r="C44" s="75"/>
+      <c r="C44" s="62"/>
       <c r="D44" s="50"/>
       <c r="E44" s="51"/>
       <c r="F44" s="34"/>
@@ -9309,7 +9309,7 @@
     <row r="45" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="34"/>
       <c r="B45" s="37"/>
-      <c r="C45" s="75"/>
+      <c r="C45" s="62"/>
       <c r="D45" s="50"/>
       <c r="E45" s="51"/>
       <c r="F45" s="34"/>
@@ -9343,7 +9343,7 @@
     <row r="46" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="34"/>
       <c r="B46" s="37"/>
-      <c r="C46" s="75"/>
+      <c r="C46" s="62"/>
       <c r="D46" s="50"/>
       <c r="E46" s="51"/>
       <c r="F46" s="34"/>
@@ -9377,7 +9377,7 @@
     <row r="47" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="34"/>
       <c r="B47" s="37"/>
-      <c r="C47" s="75"/>
+      <c r="C47" s="62"/>
       <c r="D47" s="50"/>
       <c r="E47" s="51"/>
       <c r="F47" s="34"/>
@@ -9411,7 +9411,7 @@
     <row r="48" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="34"/>
       <c r="B48" s="37"/>
-      <c r="C48" s="75"/>
+      <c r="C48" s="62"/>
       <c r="D48" s="50"/>
       <c r="E48" s="51"/>
       <c r="F48" s="34"/>
@@ -9445,7 +9445,7 @@
     <row r="49" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="34"/>
       <c r="B49" s="37"/>
-      <c r="C49" s="75"/>
+      <c r="C49" s="62"/>
       <c r="D49" s="50"/>
       <c r="E49" s="51"/>
       <c r="F49" s="34"/>
@@ -9479,7 +9479,7 @@
     <row r="50" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="34"/>
       <c r="B50" s="37"/>
-      <c r="C50" s="75"/>
+      <c r="C50" s="62"/>
       <c r="D50" s="50"/>
       <c r="E50" s="51"/>
       <c r="F50" s="34"/>
@@ -9513,7 +9513,7 @@
     <row r="51" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="34"/>
       <c r="B51" s="37"/>
-      <c r="C51" s="75"/>
+      <c r="C51" s="62"/>
       <c r="D51" s="50"/>
       <c r="E51" s="51"/>
       <c r="F51" s="34"/>
@@ -9547,7 +9547,7 @@
     <row r="52" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="34"/>
       <c r="B52" s="37"/>
-      <c r="C52" s="75"/>
+      <c r="C52" s="62"/>
       <c r="D52" s="50"/>
       <c r="E52" s="51"/>
       <c r="F52" s="34"/>
@@ -9581,7 +9581,7 @@
     <row r="53" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="34"/>
       <c r="B53" s="37"/>
-      <c r="C53" s="75"/>
+      <c r="C53" s="62"/>
       <c r="D53" s="50"/>
       <c r="E53" s="51"/>
       <c r="F53" s="34"/>
@@ -9615,7 +9615,7 @@
     <row r="54" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="34"/>
       <c r="B54" s="37"/>
-      <c r="C54" s="75"/>
+      <c r="C54" s="62"/>
       <c r="D54" s="50"/>
       <c r="E54" s="51"/>
       <c r="F54" s="34"/>
@@ -9649,7 +9649,7 @@
     <row r="55" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="34"/>
       <c r="B55" s="37"/>
-      <c r="C55" s="75"/>
+      <c r="C55" s="62"/>
       <c r="D55" s="50"/>
       <c r="E55" s="51"/>
       <c r="F55" s="34"/>
@@ -9683,7 +9683,7 @@
     <row r="56" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="34"/>
       <c r="B56" s="37"/>
-      <c r="C56" s="75"/>
+      <c r="C56" s="62"/>
       <c r="D56" s="50"/>
       <c r="E56" s="51"/>
       <c r="F56" s="34"/>
@@ -9717,7 +9717,7 @@
     <row r="57" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="34"/>
       <c r="B57" s="37"/>
-      <c r="C57" s="75"/>
+      <c r="C57" s="62"/>
       <c r="D57" s="50"/>
       <c r="E57" s="51"/>
       <c r="F57" s="34"/>
@@ -9751,7 +9751,7 @@
     <row r="58" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="34"/>
       <c r="B58" s="34"/>
-      <c r="C58" s="76"/>
+      <c r="C58" s="61"/>
       <c r="D58" s="50"/>
       <c r="E58" s="51"/>
       <c r="F58" s="34"/>
@@ -9785,7 +9785,7 @@
     <row r="59" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="34"/>
       <c r="B59" s="34"/>
-      <c r="C59" s="76"/>
+      <c r="C59" s="61"/>
       <c r="D59" s="50"/>
       <c r="E59" s="51"/>
       <c r="F59" s="34"/>
@@ -9819,7 +9819,7 @@
     <row r="60" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="34"/>
       <c r="B60" s="34"/>
-      <c r="C60" s="76"/>
+      <c r="C60" s="61"/>
       <c r="D60" s="50"/>
       <c r="E60" s="51"/>
       <c r="F60" s="34"/>
@@ -9853,7 +9853,7 @@
     <row r="61" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="34"/>
       <c r="B61" s="34"/>
-      <c r="C61" s="76"/>
+      <c r="C61" s="61"/>
       <c r="D61" s="50"/>
       <c r="E61" s="51"/>
       <c r="F61" s="34"/>
@@ -9887,7 +9887,7 @@
     <row r="62" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="34"/>
       <c r="B62" s="34"/>
-      <c r="C62" s="76"/>
+      <c r="C62" s="61"/>
       <c r="D62" s="50"/>
       <c r="E62" s="51"/>
       <c r="F62" s="34"/>
@@ -9921,7 +9921,7 @@
     <row r="63" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="34"/>
       <c r="B63" s="34"/>
-      <c r="C63" s="76"/>
+      <c r="C63" s="61"/>
       <c r="D63" s="50"/>
       <c r="E63" s="51"/>
       <c r="F63" s="34"/>
@@ -9955,7 +9955,7 @@
     <row r="64" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="34"/>
       <c r="B64" s="34"/>
-      <c r="C64" s="76"/>
+      <c r="C64" s="61"/>
       <c r="D64" s="50"/>
       <c r="E64" s="51"/>
       <c r="F64" s="34"/>
@@ -9989,7 +9989,7 @@
     <row r="65" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="34"/>
       <c r="B65" s="34"/>
-      <c r="C65" s="76"/>
+      <c r="C65" s="61"/>
       <c r="D65" s="50"/>
       <c r="E65" s="51"/>
       <c r="F65" s="34"/>
@@ -10023,7 +10023,7 @@
     <row r="66" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="34"/>
       <c r="B66" s="34"/>
-      <c r="C66" s="76"/>
+      <c r="C66" s="61"/>
       <c r="D66" s="50"/>
       <c r="E66" s="51"/>
       <c r="F66" s="34"/>
@@ -10057,7 +10057,7 @@
     <row r="67" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="34"/>
       <c r="B67" s="34"/>
-      <c r="C67" s="76"/>
+      <c r="C67" s="61"/>
       <c r="D67" s="50"/>
       <c r="E67" s="51"/>
       <c r="F67" s="34"/>
@@ -10091,7 +10091,7 @@
     <row r="68" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="34"/>
       <c r="B68" s="34"/>
-      <c r="C68" s="76"/>
+      <c r="C68" s="61"/>
       <c r="D68" s="50"/>
       <c r="E68" s="51"/>
       <c r="F68" s="34"/>
@@ -10125,7 +10125,7 @@
     <row r="69" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="34"/>
       <c r="B69" s="34"/>
-      <c r="C69" s="76"/>
+      <c r="C69" s="61"/>
       <c r="D69" s="50"/>
       <c r="E69" s="51"/>
       <c r="F69" s="34"/>
@@ -10159,7 +10159,7 @@
     <row r="70" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="34"/>
       <c r="B70" s="34"/>
-      <c r="C70" s="76"/>
+      <c r="C70" s="61"/>
       <c r="D70" s="50"/>
       <c r="E70" s="51"/>
       <c r="F70" s="34"/>
@@ -10193,7 +10193,7 @@
     <row r="71" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="34"/>
       <c r="B71" s="34"/>
-      <c r="C71" s="76"/>
+      <c r="C71" s="61"/>
       <c r="D71" s="50"/>
       <c r="E71" s="51"/>
       <c r="F71" s="34"/>
@@ -10227,7 +10227,7 @@
     <row r="72" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="34"/>
       <c r="B72" s="34"/>
-      <c r="C72" s="76"/>
+      <c r="C72" s="61"/>
       <c r="D72" s="50"/>
       <c r="E72" s="51"/>
       <c r="F72" s="34"/>
@@ -10261,7 +10261,7 @@
     <row r="73" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="34"/>
       <c r="B73" s="34"/>
-      <c r="C73" s="76"/>
+      <c r="C73" s="61"/>
       <c r="D73" s="50"/>
       <c r="E73" s="51"/>
       <c r="F73" s="34"/>
@@ -10295,7 +10295,7 @@
     <row r="74" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="34"/>
       <c r="B74" s="34"/>
-      <c r="C74" s="76"/>
+      <c r="C74" s="61"/>
       <c r="D74" s="50"/>
       <c r="E74" s="51"/>
       <c r="F74" s="34"/>
@@ -10329,7 +10329,7 @@
     <row r="75" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="34"/>
       <c r="B75" s="34"/>
-      <c r="C75" s="76"/>
+      <c r="C75" s="61"/>
       <c r="D75" s="50"/>
       <c r="E75" s="51"/>
       <c r="F75" s="34"/>
@@ -10363,7 +10363,7 @@
     <row r="76" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="34"/>
       <c r="B76" s="34"/>
-      <c r="C76" s="76"/>
+      <c r="C76" s="61"/>
       <c r="D76" s="50"/>
       <c r="E76" s="51"/>
       <c r="F76" s="34"/>
@@ -10397,7 +10397,7 @@
     <row r="77" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="34"/>
       <c r="B77" s="34"/>
-      <c r="C77" s="76"/>
+      <c r="C77" s="61"/>
       <c r="D77" s="50"/>
       <c r="E77" s="51"/>
       <c r="F77" s="34"/>
@@ -10431,7 +10431,7 @@
     <row r="78" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="34"/>
       <c r="B78" s="34"/>
-      <c r="C78" s="76"/>
+      <c r="C78" s="61"/>
       <c r="D78" s="50"/>
       <c r="E78" s="51"/>
       <c r="F78" s="34"/>
@@ -10465,7 +10465,7 @@
     <row r="79" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="34"/>
       <c r="B79" s="34"/>
-      <c r="C79" s="76"/>
+      <c r="C79" s="61"/>
       <c r="D79" s="50"/>
       <c r="E79" s="51"/>
       <c r="F79" s="34"/>
@@ -10499,7 +10499,7 @@
     <row r="80" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="34"/>
       <c r="B80" s="34"/>
-      <c r="C80" s="76"/>
+      <c r="C80" s="61"/>
       <c r="D80" s="50"/>
       <c r="E80" s="51"/>
       <c r="F80" s="34"/>
@@ -10533,7 +10533,7 @@
     <row r="81" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="34"/>
       <c r="B81" s="34"/>
-      <c r="C81" s="76"/>
+      <c r="C81" s="61"/>
       <c r="D81" s="50"/>
       <c r="E81" s="51"/>
       <c r="F81" s="34"/>
@@ -10567,7 +10567,7 @@
     <row r="82" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="34"/>
       <c r="B82" s="34"/>
-      <c r="C82" s="76"/>
+      <c r="C82" s="61"/>
       <c r="D82" s="50"/>
       <c r="E82" s="51"/>
       <c r="F82" s="34"/>
@@ -10601,7 +10601,7 @@
     <row r="83" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="34"/>
       <c r="B83" s="34"/>
-      <c r="C83" s="76"/>
+      <c r="C83" s="61"/>
       <c r="D83" s="50"/>
       <c r="E83" s="51"/>
       <c r="F83" s="34"/>
@@ -10635,7 +10635,7 @@
     <row r="84" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="34"/>
       <c r="B84" s="34"/>
-      <c r="C84" s="76"/>
+      <c r="C84" s="61"/>
       <c r="D84" s="50"/>
       <c r="E84" s="51"/>
       <c r="F84" s="34"/>
@@ -10669,7 +10669,7 @@
     <row r="85" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="34"/>
       <c r="B85" s="34"/>
-      <c r="C85" s="76"/>
+      <c r="C85" s="61"/>
       <c r="D85" s="50"/>
       <c r="E85" s="51"/>
       <c r="F85" s="34"/>
@@ -10703,7 +10703,7 @@
     <row r="86" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="34"/>
       <c r="B86" s="34"/>
-      <c r="C86" s="76"/>
+      <c r="C86" s="61"/>
       <c r="D86" s="50"/>
       <c r="E86" s="51"/>
       <c r="F86" s="34"/>
@@ -10737,7 +10737,7 @@
     <row r="87" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="34"/>
       <c r="B87" s="34"/>
-      <c r="C87" s="76"/>
+      <c r="C87" s="61"/>
       <c r="D87" s="50"/>
       <c r="E87" s="51"/>
       <c r="F87" s="34"/>
@@ -10771,7 +10771,7 @@
     <row r="88" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="34"/>
       <c r="B88" s="34"/>
-      <c r="C88" s="76"/>
+      <c r="C88" s="61"/>
       <c r="D88" s="50"/>
       <c r="E88" s="51"/>
       <c r="F88" s="34"/>
@@ -10805,7 +10805,7 @@
     <row r="89" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="34"/>
       <c r="B89" s="34"/>
-      <c r="C89" s="76"/>
+      <c r="C89" s="61"/>
       <c r="D89" s="50"/>
       <c r="E89" s="51"/>
       <c r="F89" s="34"/>
@@ -10839,7 +10839,7 @@
     <row r="90" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="34"/>
       <c r="B90" s="34"/>
-      <c r="C90" s="76"/>
+      <c r="C90" s="61"/>
       <c r="D90" s="50"/>
       <c r="E90" s="51"/>
       <c r="F90" s="34"/>
@@ -10873,7 +10873,7 @@
     <row r="91" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="34"/>
       <c r="B91" s="34"/>
-      <c r="C91" s="76"/>
+      <c r="C91" s="61"/>
       <c r="D91" s="50"/>
       <c r="E91" s="51"/>
       <c r="F91" s="34"/>
@@ -10907,7 +10907,7 @@
     <row r="92" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="34"/>
       <c r="B92" s="34"/>
-      <c r="C92" s="76"/>
+      <c r="C92" s="61"/>
       <c r="D92" s="50"/>
       <c r="E92" s="51"/>
       <c r="F92" s="34"/>
@@ -10941,7 +10941,7 @@
     <row r="93" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="34"/>
       <c r="B93" s="34"/>
-      <c r="C93" s="76"/>
+      <c r="C93" s="61"/>
       <c r="D93" s="50"/>
       <c r="E93" s="51"/>
       <c r="F93" s="34"/>
@@ -10975,7 +10975,7 @@
     <row r="94" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="34"/>
       <c r="B94" s="34"/>
-      <c r="C94" s="76"/>
+      <c r="C94" s="61"/>
       <c r="D94" s="50"/>
       <c r="E94" s="51"/>
       <c r="F94" s="34"/>
@@ -11009,7 +11009,7 @@
     <row r="95" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="34"/>
       <c r="B95" s="34"/>
-      <c r="C95" s="76"/>
+      <c r="C95" s="61"/>
       <c r="D95" s="50"/>
       <c r="E95" s="51"/>
       <c r="F95" s="34"/>
@@ -11043,7 +11043,7 @@
     <row r="96" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="34"/>
       <c r="B96" s="34"/>
-      <c r="C96" s="76"/>
+      <c r="C96" s="61"/>
       <c r="D96" s="50"/>
       <c r="E96" s="51"/>
       <c r="F96" s="34"/>
@@ -11077,7 +11077,7 @@
     <row r="97" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="34"/>
       <c r="B97" s="34"/>
-      <c r="C97" s="76"/>
+      <c r="C97" s="61"/>
       <c r="D97" s="50"/>
       <c r="E97" s="51"/>
       <c r="F97" s="34"/>
@@ -11111,7 +11111,7 @@
     <row r="98" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="34"/>
       <c r="B98" s="34"/>
-      <c r="C98" s="76"/>
+      <c r="C98" s="61"/>
       <c r="D98" s="50"/>
       <c r="E98" s="51"/>
       <c r="F98" s="34"/>
@@ -11145,7 +11145,7 @@
     <row r="99" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="34"/>
       <c r="B99" s="34"/>
-      <c r="C99" s="76"/>
+      <c r="C99" s="61"/>
       <c r="D99" s="50"/>
       <c r="E99" s="51"/>
       <c r="F99" s="34"/>
@@ -11179,7 +11179,7 @@
     <row r="100" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="34"/>
       <c r="B100" s="34"/>
-      <c r="C100" s="76"/>
+      <c r="C100" s="61"/>
       <c r="D100" s="50"/>
       <c r="E100" s="51"/>
       <c r="F100" s="34"/>
@@ -11213,7 +11213,7 @@
     <row r="101" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="34"/>
       <c r="B101" s="34"/>
-      <c r="C101" s="76"/>
+      <c r="C101" s="61"/>
       <c r="D101" s="50"/>
       <c r="E101" s="51"/>
       <c r="F101" s="34"/>
@@ -11247,7 +11247,7 @@
     <row r="102" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
       <c r="B102" s="34"/>
-      <c r="C102" s="76"/>
+      <c r="C102" s="61"/>
       <c r="D102" s="50"/>
       <c r="E102" s="51"/>
       <c r="F102" s="34"/>
@@ -11281,7 +11281,7 @@
     <row r="103" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="34"/>
       <c r="B103" s="34"/>
-      <c r="C103" s="76"/>
+      <c r="C103" s="61"/>
       <c r="D103" s="50"/>
       <c r="E103" s="51"/>
       <c r="F103" s="34"/>
@@ -11315,7 +11315,7 @@
     <row r="104" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="34"/>
       <c r="B104" s="34"/>
-      <c r="C104" s="76"/>
+      <c r="C104" s="61"/>
       <c r="D104" s="50"/>
       <c r="E104" s="51"/>
       <c r="F104" s="34"/>
@@ -11349,7 +11349,7 @@
     <row r="105" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="34"/>
       <c r="B105" s="34"/>
-      <c r="C105" s="76"/>
+      <c r="C105" s="61"/>
       <c r="D105" s="50"/>
       <c r="E105" s="51"/>
       <c r="F105" s="34"/>
@@ -11383,7 +11383,7 @@
     <row r="106" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="34"/>
       <c r="B106" s="34"/>
-      <c r="C106" s="76"/>
+      <c r="C106" s="61"/>
       <c r="D106" s="50"/>
       <c r="E106" s="51"/>
       <c r="F106" s="34"/>
@@ -11417,7 +11417,7 @@
     <row r="107" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="34"/>
       <c r="B107" s="34"/>
-      <c r="C107" s="76"/>
+      <c r="C107" s="61"/>
       <c r="D107" s="50"/>
       <c r="E107" s="51"/>
       <c r="F107" s="34"/>
@@ -11451,7 +11451,7 @@
     <row r="108" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="34"/>
       <c r="B108" s="34"/>
-      <c r="C108" s="76"/>
+      <c r="C108" s="61"/>
       <c r="D108" s="50"/>
       <c r="E108" s="51"/>
       <c r="F108" s="34"/>
@@ -11485,7 +11485,7 @@
     <row r="109" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="34"/>
       <c r="B109" s="34"/>
-      <c r="C109" s="76"/>
+      <c r="C109" s="61"/>
       <c r="D109" s="50"/>
       <c r="E109" s="51"/>
       <c r="F109" s="34"/>
@@ -11519,7 +11519,7 @@
     <row r="110" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="34"/>
       <c r="B110" s="34"/>
-      <c r="C110" s="76"/>
+      <c r="C110" s="61"/>
       <c r="D110" s="50"/>
       <c r="E110" s="51"/>
       <c r="F110" s="34"/>
@@ -11553,7 +11553,7 @@
     <row r="111" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="34"/>
       <c r="B111" s="34"/>
-      <c r="C111" s="76"/>
+      <c r="C111" s="61"/>
       <c r="D111" s="50"/>
       <c r="E111" s="51"/>
       <c r="F111" s="34"/>
@@ -11587,7 +11587,7 @@
     <row r="112" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="34"/>
       <c r="B112" s="34"/>
-      <c r="C112" s="76"/>
+      <c r="C112" s="61"/>
       <c r="D112" s="50"/>
       <c r="E112" s="51"/>
       <c r="F112" s="34"/>
@@ -11621,7 +11621,7 @@
     <row r="113" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="34"/>
       <c r="B113" s="34"/>
-      <c r="C113" s="76"/>
+      <c r="C113" s="61"/>
       <c r="D113" s="50"/>
       <c r="E113" s="51"/>
       <c r="F113" s="34"/>
@@ -11655,7 +11655,7 @@
     <row r="114" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="34"/>
       <c r="B114" s="34"/>
-      <c r="C114" s="76"/>
+      <c r="C114" s="61"/>
       <c r="D114" s="50"/>
       <c r="E114" s="51"/>
       <c r="F114" s="34"/>
@@ -11689,7 +11689,7 @@
     <row r="115" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="34"/>
       <c r="B115" s="34"/>
-      <c r="C115" s="76"/>
+      <c r="C115" s="61"/>
       <c r="D115" s="50"/>
       <c r="E115" s="51"/>
       <c r="F115" s="34"/>
@@ -11723,7 +11723,7 @@
     <row r="116" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="34"/>
       <c r="B116" s="34"/>
-      <c r="C116" s="76"/>
+      <c r="C116" s="61"/>
       <c r="D116" s="50"/>
       <c r="E116" s="51"/>
       <c r="F116" s="34"/>
@@ -11757,7 +11757,7 @@
     <row r="117" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="34"/>
       <c r="B117" s="34"/>
-      <c r="C117" s="76"/>
+      <c r="C117" s="61"/>
       <c r="D117" s="50"/>
       <c r="E117" s="51"/>
       <c r="F117" s="34"/>
@@ -11791,7 +11791,7 @@
     <row r="118" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="34"/>
       <c r="B118" s="34"/>
-      <c r="C118" s="76"/>
+      <c r="C118" s="61"/>
       <c r="D118" s="50"/>
       <c r="E118" s="51"/>
       <c r="F118" s="34"/>
@@ -11825,7 +11825,7 @@
     <row r="119" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="34"/>
       <c r="B119" s="34"/>
-      <c r="C119" s="76"/>
+      <c r="C119" s="61"/>
       <c r="D119" s="50"/>
       <c r="E119" s="51"/>
       <c r="F119" s="34"/>
@@ -11859,7 +11859,7 @@
     <row r="120" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="34"/>
       <c r="B120" s="34"/>
-      <c r="C120" s="76"/>
+      <c r="C120" s="61"/>
       <c r="D120" s="50"/>
       <c r="E120" s="51"/>
       <c r="F120" s="34"/>
@@ -11893,7 +11893,7 @@
     <row r="121" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="34"/>
       <c r="B121" s="34"/>
-      <c r="C121" s="76"/>
+      <c r="C121" s="61"/>
       <c r="D121" s="50"/>
       <c r="E121" s="51"/>
       <c r="F121" s="34"/>
@@ -11927,7 +11927,7 @@
     <row r="122" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="34"/>
       <c r="B122" s="34"/>
-      <c r="C122" s="76"/>
+      <c r="C122" s="61"/>
       <c r="D122" s="50"/>
       <c r="E122" s="51"/>
       <c r="F122" s="34"/>
@@ -11961,7 +11961,7 @@
     <row r="123" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="34"/>
       <c r="B123" s="34"/>
-      <c r="C123" s="76"/>
+      <c r="C123" s="61"/>
       <c r="D123" s="50"/>
       <c r="E123" s="51"/>
       <c r="F123" s="34"/>
@@ -11995,7 +11995,7 @@
     <row r="124" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="34"/>
       <c r="B124" s="34"/>
-      <c r="C124" s="76"/>
+      <c r="C124" s="61"/>
       <c r="D124" s="50"/>
       <c r="E124" s="51"/>
       <c r="F124" s="34"/>
@@ -12029,7 +12029,7 @@
     <row r="125" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="34"/>
       <c r="B125" s="34"/>
-      <c r="C125" s="76"/>
+      <c r="C125" s="61"/>
       <c r="D125" s="50"/>
       <c r="E125" s="51"/>
       <c r="F125" s="34"/>
@@ -12063,7 +12063,7 @@
     <row r="126" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="34"/>
       <c r="B126" s="34"/>
-      <c r="C126" s="76"/>
+      <c r="C126" s="61"/>
       <c r="D126" s="50"/>
       <c r="E126" s="51"/>
       <c r="F126" s="34"/>
@@ -12097,7 +12097,7 @@
     <row r="127" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="34"/>
       <c r="B127" s="34"/>
-      <c r="C127" s="76"/>
+      <c r="C127" s="61"/>
       <c r="D127" s="50"/>
       <c r="E127" s="51"/>
       <c r="F127" s="34"/>
@@ -12131,7 +12131,7 @@
     <row r="128" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="34"/>
       <c r="B128" s="34"/>
-      <c r="C128" s="76"/>
+      <c r="C128" s="61"/>
       <c r="D128" s="50"/>
       <c r="E128" s="51"/>
       <c r="F128" s="34"/>
@@ -12165,7 +12165,7 @@
     <row r="129" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="34"/>
       <c r="B129" s="34"/>
-      <c r="C129" s="76"/>
+      <c r="C129" s="61"/>
       <c r="D129" s="50"/>
       <c r="E129" s="51"/>
       <c r="F129" s="34"/>
@@ -12199,7 +12199,7 @@
     <row r="130" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="34"/>
       <c r="B130" s="34"/>
-      <c r="C130" s="76"/>
+      <c r="C130" s="61"/>
       <c r="D130" s="50"/>
       <c r="E130" s="51"/>
       <c r="F130" s="34"/>
@@ -12233,7 +12233,7 @@
     <row r="131" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="34"/>
       <c r="B131" s="34"/>
-      <c r="C131" s="76"/>
+      <c r="C131" s="61"/>
       <c r="D131" s="50"/>
       <c r="E131" s="51"/>
       <c r="F131" s="34"/>
@@ -12267,7 +12267,7 @@
     <row r="132" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="34"/>
       <c r="B132" s="34"/>
-      <c r="C132" s="76"/>
+      <c r="C132" s="61"/>
       <c r="D132" s="50"/>
       <c r="E132" s="51"/>
       <c r="F132" s="34"/>
@@ -12301,7 +12301,7 @@
     <row r="133" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="34"/>
       <c r="B133" s="34"/>
-      <c r="C133" s="76"/>
+      <c r="C133" s="61"/>
       <c r="D133" s="50"/>
       <c r="E133" s="51"/>
       <c r="F133" s="34"/>
@@ -12335,7 +12335,7 @@
     <row r="134" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="34"/>
       <c r="B134" s="34"/>
-      <c r="C134" s="76"/>
+      <c r="C134" s="61"/>
       <c r="D134" s="50"/>
       <c r="E134" s="51"/>
       <c r="F134" s="34"/>
@@ -12369,7 +12369,7 @@
     <row r="135" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="34"/>
       <c r="B135" s="34"/>
-      <c r="C135" s="76"/>
+      <c r="C135" s="61"/>
       <c r="D135" s="50"/>
       <c r="E135" s="51"/>
       <c r="F135" s="34"/>
@@ -12403,7 +12403,7 @@
     <row r="136" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="34"/>
       <c r="B136" s="34"/>
-      <c r="C136" s="76"/>
+      <c r="C136" s="61"/>
       <c r="D136" s="50"/>
       <c r="E136" s="51"/>
       <c r="F136" s="34"/>
@@ -12437,7 +12437,7 @@
     <row r="137" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="34"/>
       <c r="B137" s="34"/>
-      <c r="C137" s="76"/>
+      <c r="C137" s="61"/>
       <c r="D137" s="50"/>
       <c r="E137" s="51"/>
       <c r="F137" s="34"/>
@@ -12471,7 +12471,7 @@
     <row r="138" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="34"/>
       <c r="B138" s="34"/>
-      <c r="C138" s="76"/>
+      <c r="C138" s="61"/>
       <c r="D138" s="50"/>
       <c r="E138" s="51"/>
       <c r="F138" s="34"/>
@@ -12505,7 +12505,7 @@
     <row r="139" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="34"/>
       <c r="B139" s="34"/>
-      <c r="C139" s="76"/>
+      <c r="C139" s="61"/>
       <c r="D139" s="50"/>
       <c r="E139" s="51"/>
       <c r="F139" s="34"/>
@@ -12539,7 +12539,7 @@
     <row r="140" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="34"/>
       <c r="B140" s="34"/>
-      <c r="C140" s="76"/>
+      <c r="C140" s="61"/>
       <c r="D140" s="50"/>
       <c r="E140" s="51"/>
       <c r="F140" s="34"/>
@@ -12573,7 +12573,7 @@
     <row r="141" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="34"/>
       <c r="B141" s="34"/>
-      <c r="C141" s="76"/>
+      <c r="C141" s="61"/>
       <c r="D141" s="50"/>
       <c r="E141" s="51"/>
       <c r="F141" s="34"/>
@@ -12607,7 +12607,7 @@
     <row r="142" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="34"/>
       <c r="B142" s="34"/>
-      <c r="C142" s="76"/>
+      <c r="C142" s="61"/>
       <c r="D142" s="50"/>
       <c r="E142" s="51"/>
       <c r="F142" s="34"/>
@@ -12641,7 +12641,7 @@
     <row r="143" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="34"/>
       <c r="B143" s="34"/>
-      <c r="C143" s="76"/>
+      <c r="C143" s="61"/>
       <c r="D143" s="50"/>
       <c r="E143" s="51"/>
       <c r="F143" s="34"/>
@@ -12675,7 +12675,7 @@
     <row r="144" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="34"/>
       <c r="B144" s="34"/>
-      <c r="C144" s="76"/>
+      <c r="C144" s="61"/>
       <c r="D144" s="50"/>
       <c r="E144" s="51"/>
       <c r="F144" s="34"/>
@@ -12709,7 +12709,7 @@
     <row r="145" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="34"/>
       <c r="B145" s="34"/>
-      <c r="C145" s="76"/>
+      <c r="C145" s="61"/>
       <c r="D145" s="50"/>
       <c r="E145" s="51"/>
       <c r="F145" s="34"/>
@@ -12743,7 +12743,7 @@
     <row r="146" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="34"/>
       <c r="B146" s="34"/>
-      <c r="C146" s="76"/>
+      <c r="C146" s="61"/>
       <c r="D146" s="50"/>
       <c r="E146" s="51"/>
       <c r="F146" s="34"/>
@@ -12777,7 +12777,7 @@
     <row r="147" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="34"/>
       <c r="B147" s="34"/>
-      <c r="C147" s="76"/>
+      <c r="C147" s="61"/>
       <c r="D147" s="50"/>
       <c r="E147" s="51"/>
       <c r="F147" s="34"/>
@@ -12811,7 +12811,7 @@
     <row r="148" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="34"/>
       <c r="B148" s="34"/>
-      <c r="C148" s="76"/>
+      <c r="C148" s="61"/>
       <c r="D148" s="50"/>
       <c r="E148" s="51"/>
       <c r="F148" s="34"/>
@@ -12845,7 +12845,7 @@
     <row r="149" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="34"/>
       <c r="B149" s="34"/>
-      <c r="C149" s="76"/>
+      <c r="C149" s="61"/>
       <c r="D149" s="50"/>
       <c r="E149" s="51"/>
       <c r="F149" s="34"/>
@@ -12879,7 +12879,7 @@
     <row r="150" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="34"/>
       <c r="B150" s="34"/>
-      <c r="C150" s="76"/>
+      <c r="C150" s="61"/>
       <c r="D150" s="50"/>
       <c r="E150" s="51"/>
       <c r="F150" s="34"/>
@@ -12913,7 +12913,7 @@
     <row r="151" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="34"/>
       <c r="B151" s="34"/>
-      <c r="C151" s="76"/>
+      <c r="C151" s="61"/>
       <c r="D151" s="50"/>
       <c r="E151" s="51"/>
       <c r="F151" s="34"/>
@@ -12947,7 +12947,7 @@
     <row r="152" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="34"/>
       <c r="B152" s="34"/>
-      <c r="C152" s="76"/>
+      <c r="C152" s="61"/>
       <c r="D152" s="50"/>
       <c r="E152" s="51"/>
       <c r="F152" s="34"/>
@@ -12981,7 +12981,7 @@
     <row r="153" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="34"/>
       <c r="B153" s="34"/>
-      <c r="C153" s="76"/>
+      <c r="C153" s="61"/>
       <c r="D153" s="50"/>
       <c r="E153" s="51"/>
       <c r="F153" s="34"/>
@@ -13015,7 +13015,7 @@
     <row r="154" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="34"/>
       <c r="B154" s="34"/>
-      <c r="C154" s="76"/>
+      <c r="C154" s="61"/>
       <c r="D154" s="50"/>
       <c r="E154" s="51"/>
       <c r="F154" s="34"/>
@@ -13049,7 +13049,7 @@
     <row r="155" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="34"/>
       <c r="B155" s="34"/>
-      <c r="C155" s="76"/>
+      <c r="C155" s="61"/>
       <c r="D155" s="50"/>
       <c r="E155" s="51"/>
       <c r="F155" s="34"/>
@@ -13083,7 +13083,7 @@
     <row r="156" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="34"/>
       <c r="B156" s="34"/>
-      <c r="C156" s="76"/>
+      <c r="C156" s="61"/>
       <c r="D156" s="50"/>
       <c r="E156" s="51"/>
       <c r="F156" s="34"/>
@@ -13117,7 +13117,7 @@
     <row r="157" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="34"/>
       <c r="B157" s="34"/>
-      <c r="C157" s="76"/>
+      <c r="C157" s="61"/>
       <c r="D157" s="50"/>
       <c r="E157" s="51"/>
       <c r="F157" s="34"/>
@@ -13151,7 +13151,7 @@
     <row r="158" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="34"/>
       <c r="B158" s="34"/>
-      <c r="C158" s="76"/>
+      <c r="C158" s="61"/>
       <c r="D158" s="50"/>
       <c r="E158" s="51"/>
       <c r="F158" s="34"/>
@@ -13185,7 +13185,7 @@
     <row r="159" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="34"/>
       <c r="B159" s="34"/>
-      <c r="C159" s="76"/>
+      <c r="C159" s="61"/>
       <c r="D159" s="50"/>
       <c r="E159" s="51"/>
       <c r="F159" s="34"/>
@@ -13219,7 +13219,7 @@
     <row r="160" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="34"/>
       <c r="B160" s="34"/>
-      <c r="C160" s="76"/>
+      <c r="C160" s="61"/>
       <c r="D160" s="50"/>
       <c r="E160" s="51"/>
       <c r="F160" s="34"/>
@@ -13253,7 +13253,7 @@
     <row r="161" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="34"/>
       <c r="B161" s="34"/>
-      <c r="C161" s="76"/>
+      <c r="C161" s="61"/>
       <c r="D161" s="50"/>
       <c r="E161" s="51"/>
       <c r="F161" s="34"/>
@@ -13287,7 +13287,7 @@
     <row r="162" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="34"/>
       <c r="B162" s="34"/>
-      <c r="C162" s="76"/>
+      <c r="C162" s="61"/>
       <c r="D162" s="50"/>
       <c r="E162" s="51"/>
       <c r="F162" s="34"/>
@@ -13321,7 +13321,7 @@
     <row r="163" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="34"/>
       <c r="B163" s="34"/>
-      <c r="C163" s="76"/>
+      <c r="C163" s="61"/>
       <c r="D163" s="50"/>
       <c r="E163" s="51"/>
       <c r="F163" s="34"/>
@@ -13355,7 +13355,7 @@
     <row r="164" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="34"/>
       <c r="B164" s="34"/>
-      <c r="C164" s="76"/>
+      <c r="C164" s="61"/>
       <c r="D164" s="50"/>
       <c r="E164" s="51"/>
       <c r="F164" s="34"/>
@@ -13389,7 +13389,7 @@
     <row r="165" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="34"/>
       <c r="B165" s="34"/>
-      <c r="C165" s="76"/>
+      <c r="C165" s="61"/>
       <c r="D165" s="50"/>
       <c r="E165" s="51"/>
       <c r="F165" s="34"/>
@@ -13423,7 +13423,7 @@
     <row r="166" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="34"/>
       <c r="B166" s="34"/>
-      <c r="C166" s="76"/>
+      <c r="C166" s="61"/>
       <c r="D166" s="50"/>
       <c r="E166" s="51"/>
       <c r="F166" s="34"/>
@@ -13457,7 +13457,7 @@
     <row r="167" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="34"/>
       <c r="B167" s="34"/>
-      <c r="C167" s="76"/>
+      <c r="C167" s="61"/>
       <c r="D167" s="50"/>
       <c r="E167" s="51"/>
       <c r="F167" s="34"/>
@@ -13491,7 +13491,7 @@
     <row r="168" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="34"/>
       <c r="B168" s="34"/>
-      <c r="C168" s="76"/>
+      <c r="C168" s="61"/>
       <c r="D168" s="50"/>
       <c r="E168" s="51"/>
       <c r="F168" s="34"/>
@@ -13525,7 +13525,7 @@
     <row r="169" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="34"/>
       <c r="B169" s="34"/>
-      <c r="C169" s="76"/>
+      <c r="C169" s="61"/>
       <c r="D169" s="50"/>
       <c r="E169" s="51"/>
       <c r="F169" s="34"/>
@@ -13559,7 +13559,7 @@
     <row r="170" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="34"/>
       <c r="B170" s="34"/>
-      <c r="C170" s="76"/>
+      <c r="C170" s="61"/>
       <c r="D170" s="50"/>
       <c r="E170" s="51"/>
       <c r="F170" s="34"/>
@@ -13593,7 +13593,7 @@
     <row r="171" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="34"/>
       <c r="B171" s="34"/>
-      <c r="C171" s="76"/>
+      <c r="C171" s="61"/>
       <c r="D171" s="50"/>
       <c r="E171" s="51"/>
       <c r="F171" s="34"/>
@@ -13627,7 +13627,7 @@
     <row r="172" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="34"/>
       <c r="B172" s="34"/>
-      <c r="C172" s="76"/>
+      <c r="C172" s="61"/>
       <c r="D172" s="50"/>
       <c r="E172" s="51"/>
       <c r="F172" s="34"/>
@@ -13661,7 +13661,7 @@
     <row r="173" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="34"/>
       <c r="B173" s="34"/>
-      <c r="C173" s="76"/>
+      <c r="C173" s="61"/>
       <c r="D173" s="50"/>
       <c r="E173" s="51"/>
       <c r="F173" s="34"/>
@@ -13695,7 +13695,7 @@
     <row r="174" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="34"/>
       <c r="B174" s="34"/>
-      <c r="C174" s="76"/>
+      <c r="C174" s="61"/>
       <c r="D174" s="50"/>
       <c r="E174" s="51"/>
       <c r="F174" s="34"/>
@@ -13729,7 +13729,7 @@
     <row r="175" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="34"/>
       <c r="B175" s="34"/>
-      <c r="C175" s="76"/>
+      <c r="C175" s="61"/>
       <c r="D175" s="50"/>
       <c r="E175" s="51"/>
       <c r="F175" s="34"/>
@@ -13763,7 +13763,7 @@
     <row r="176" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="34"/>
       <c r="B176" s="34"/>
-      <c r="C176" s="76"/>
+      <c r="C176" s="61"/>
       <c r="D176" s="50"/>
       <c r="E176" s="51"/>
       <c r="F176" s="34"/>
@@ -13797,7 +13797,7 @@
     <row r="177" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="34"/>
       <c r="B177" s="34"/>
-      <c r="C177" s="76"/>
+      <c r="C177" s="61"/>
       <c r="D177" s="50"/>
       <c r="E177" s="51"/>
       <c r="F177" s="34"/>
@@ -13831,7 +13831,7 @@
     <row r="178" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="34"/>
       <c r="B178" s="34"/>
-      <c r="C178" s="76"/>
+      <c r="C178" s="61"/>
       <c r="D178" s="50"/>
       <c r="E178" s="51"/>
       <c r="F178" s="34"/>
@@ -13865,7 +13865,7 @@
     <row r="179" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="34"/>
       <c r="B179" s="34"/>
-      <c r="C179" s="76"/>
+      <c r="C179" s="61"/>
       <c r="D179" s="50"/>
       <c r="E179" s="51"/>
       <c r="F179" s="34"/>
@@ -13899,7 +13899,7 @@
     <row r="180" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="34"/>
       <c r="B180" s="34"/>
-      <c r="C180" s="76"/>
+      <c r="C180" s="61"/>
       <c r="D180" s="50"/>
       <c r="E180" s="51"/>
       <c r="F180" s="34"/>
@@ -13933,7 +13933,7 @@
     <row r="181" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="34"/>
       <c r="B181" s="34"/>
-      <c r="C181" s="76"/>
+      <c r="C181" s="61"/>
       <c r="D181" s="50"/>
       <c r="E181" s="51"/>
       <c r="F181" s="34"/>
@@ -13967,7 +13967,7 @@
     <row r="182" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="34"/>
       <c r="B182" s="34"/>
-      <c r="C182" s="76"/>
+      <c r="C182" s="61"/>
       <c r="D182" s="50"/>
       <c r="E182" s="51"/>
       <c r="F182" s="34"/>
@@ -14001,7 +14001,7 @@
     <row r="183" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="34"/>
       <c r="B183" s="34"/>
-      <c r="C183" s="76"/>
+      <c r="C183" s="61"/>
       <c r="D183" s="50"/>
       <c r="E183" s="51"/>
       <c r="F183" s="34"/>
@@ -14035,7 +14035,7 @@
     <row r="184" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="34"/>
       <c r="B184" s="34"/>
-      <c r="C184" s="76"/>
+      <c r="C184" s="61"/>
       <c r="D184" s="50"/>
       <c r="E184" s="51"/>
       <c r="F184" s="34"/>
@@ -14069,7 +14069,7 @@
     <row r="185" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="34"/>
       <c r="B185" s="34"/>
-      <c r="C185" s="76"/>
+      <c r="C185" s="61"/>
       <c r="D185" s="50"/>
       <c r="E185" s="51"/>
       <c r="F185" s="34"/>
@@ -14103,7 +14103,7 @@
     <row r="186" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="34"/>
       <c r="B186" s="34"/>
-      <c r="C186" s="76"/>
+      <c r="C186" s="61"/>
       <c r="D186" s="50"/>
       <c r="E186" s="51"/>
       <c r="F186" s="34"/>
@@ -14137,7 +14137,7 @@
     <row r="187" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="34"/>
       <c r="B187" s="34"/>
-      <c r="C187" s="76"/>
+      <c r="C187" s="61"/>
       <c r="D187" s="50"/>
       <c r="E187" s="51"/>
       <c r="F187" s="34"/>
@@ -14171,7 +14171,7 @@
     <row r="188" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="34"/>
       <c r="B188" s="34"/>
-      <c r="C188" s="76"/>
+      <c r="C188" s="61"/>
       <c r="D188" s="50"/>
       <c r="E188" s="51"/>
       <c r="F188" s="34"/>
@@ -14205,7 +14205,7 @@
     <row r="189" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="34"/>
       <c r="B189" s="34"/>
-      <c r="C189" s="76"/>
+      <c r="C189" s="61"/>
       <c r="D189" s="50"/>
       <c r="E189" s="51"/>
       <c r="F189" s="34"/>
@@ -14239,7 +14239,7 @@
     <row r="190" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="34"/>
       <c r="B190" s="34"/>
-      <c r="C190" s="76"/>
+      <c r="C190" s="61"/>
       <c r="D190" s="50"/>
       <c r="E190" s="51"/>
       <c r="F190" s="34"/>
@@ -14273,7 +14273,7 @@
     <row r="191" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="34"/>
       <c r="B191" s="34"/>
-      <c r="C191" s="76"/>
+      <c r="C191" s="61"/>
       <c r="D191" s="50"/>
       <c r="E191" s="51"/>
       <c r="F191" s="34"/>
@@ -14307,7 +14307,7 @@
     <row r="192" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="34"/>
       <c r="B192" s="34"/>
-      <c r="C192" s="76"/>
+      <c r="C192" s="61"/>
       <c r="D192" s="50"/>
       <c r="E192" s="51"/>
       <c r="F192" s="34"/>
@@ -14341,7 +14341,7 @@
     <row r="193" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="34"/>
       <c r="B193" s="34"/>
-      <c r="C193" s="76"/>
+      <c r="C193" s="61"/>
       <c r="D193" s="50"/>
       <c r="E193" s="51"/>
       <c r="F193" s="34"/>
@@ -14375,7 +14375,7 @@
     <row r="194" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="34"/>
       <c r="B194" s="34"/>
-      <c r="C194" s="76"/>
+      <c r="C194" s="61"/>
       <c r="D194" s="50"/>
       <c r="E194" s="51"/>
       <c r="F194" s="34"/>
@@ -14409,7 +14409,7 @@
     <row r="195" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="34"/>
       <c r="B195" s="34"/>
-      <c r="C195" s="76"/>
+      <c r="C195" s="61"/>
       <c r="D195" s="50"/>
       <c r="E195" s="51"/>
       <c r="F195" s="34"/>
@@ -14443,7 +14443,7 @@
     <row r="196" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="34"/>
       <c r="B196" s="34"/>
-      <c r="C196" s="76"/>
+      <c r="C196" s="61"/>
       <c r="D196" s="50"/>
       <c r="E196" s="51"/>
       <c r="F196" s="34"/>
@@ -14477,7 +14477,7 @@
     <row r="197" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="34"/>
       <c r="B197" s="34"/>
-      <c r="C197" s="76"/>
+      <c r="C197" s="61"/>
       <c r="D197" s="50"/>
       <c r="E197" s="51"/>
       <c r="F197" s="34"/>
@@ -14511,7 +14511,7 @@
     <row r="198" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="34"/>
       <c r="B198" s="34"/>
-      <c r="C198" s="76"/>
+      <c r="C198" s="61"/>
       <c r="D198" s="50"/>
       <c r="E198" s="51"/>
       <c r="F198" s="34"/>
@@ -14545,7 +14545,7 @@
     <row r="199" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="34"/>
       <c r="B199" s="34"/>
-      <c r="C199" s="76"/>
+      <c r="C199" s="61"/>
       <c r="D199" s="50"/>
       <c r="E199" s="51"/>
       <c r="F199" s="34"/>
@@ -14579,7 +14579,7 @@
     <row r="200" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="34"/>
       <c r="B200" s="34"/>
-      <c r="C200" s="76"/>
+      <c r="C200" s="61"/>
       <c r="D200" s="50"/>
       <c r="E200" s="51"/>
       <c r="F200" s="34"/>
@@ -14613,7 +14613,7 @@
     <row r="201" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="34"/>
       <c r="B201" s="34"/>
-      <c r="C201" s="76"/>
+      <c r="C201" s="61"/>
       <c r="D201" s="50"/>
       <c r="E201" s="51"/>
       <c r="F201" s="34"/>
@@ -14647,7 +14647,7 @@
     <row r="202" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="34"/>
       <c r="B202" s="34"/>
-      <c r="C202" s="76"/>
+      <c r="C202" s="61"/>
       <c r="D202" s="50"/>
       <c r="E202" s="51"/>
       <c r="F202" s="34"/>
@@ -14681,7 +14681,7 @@
     <row r="203" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="34"/>
       <c r="B203" s="34"/>
-      <c r="C203" s="76"/>
+      <c r="C203" s="61"/>
       <c r="D203" s="50"/>
       <c r="E203" s="51"/>
       <c r="F203" s="34"/>
@@ -14715,7 +14715,7 @@
     <row r="204" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="34"/>
       <c r="B204" s="34"/>
-      <c r="C204" s="76"/>
+      <c r="C204" s="61"/>
       <c r="D204" s="50"/>
       <c r="E204" s="51"/>
       <c r="F204" s="34"/>
@@ -14749,7 +14749,7 @@
     <row r="205" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="34"/>
       <c r="B205" s="34"/>
-      <c r="C205" s="76"/>
+      <c r="C205" s="61"/>
       <c r="D205" s="50"/>
       <c r="E205" s="51"/>
       <c r="F205" s="34"/>
@@ -14783,7 +14783,7 @@
     <row r="206" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="34"/>
       <c r="B206" s="34"/>
-      <c r="C206" s="76"/>
+      <c r="C206" s="61"/>
       <c r="D206" s="50"/>
       <c r="E206" s="51"/>
       <c r="F206" s="34"/>
@@ -14817,7 +14817,7 @@
     <row r="207" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="34"/>
       <c r="B207" s="34"/>
-      <c r="C207" s="76"/>
+      <c r="C207" s="61"/>
       <c r="D207" s="50"/>
       <c r="E207" s="51"/>
       <c r="F207" s="34"/>
@@ -14851,7 +14851,7 @@
     <row r="208" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="34"/>
       <c r="B208" s="34"/>
-      <c r="C208" s="76"/>
+      <c r="C208" s="61"/>
       <c r="D208" s="50"/>
       <c r="E208" s="51"/>
       <c r="F208" s="34"/>
@@ -14885,7 +14885,7 @@
     <row r="209" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="34"/>
       <c r="B209" s="34"/>
-      <c r="C209" s="76"/>
+      <c r="C209" s="61"/>
       <c r="D209" s="50"/>
       <c r="E209" s="51"/>
       <c r="F209" s="34"/>
@@ -14919,7 +14919,7 @@
     <row r="210" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="34"/>
       <c r="B210" s="34"/>
-      <c r="C210" s="76"/>
+      <c r="C210" s="61"/>
       <c r="D210" s="50"/>
       <c r="E210" s="51"/>
       <c r="F210" s="34"/>
@@ -14953,7 +14953,7 @@
     <row r="211" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="34"/>
       <c r="B211" s="34"/>
-      <c r="C211" s="76"/>
+      <c r="C211" s="61"/>
       <c r="D211" s="50"/>
       <c r="E211" s="51"/>
       <c r="F211" s="34"/>
@@ -14987,7 +14987,7 @@
     <row r="212" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="34"/>
       <c r="B212" s="34"/>
-      <c r="C212" s="76"/>
+      <c r="C212" s="61"/>
       <c r="D212" s="50"/>
       <c r="E212" s="51"/>
       <c r="F212" s="34"/>
@@ -15021,7 +15021,7 @@
     <row r="213" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="34"/>
       <c r="B213" s="34"/>
-      <c r="C213" s="76"/>
+      <c r="C213" s="61"/>
       <c r="D213" s="50"/>
       <c r="E213" s="51"/>
       <c r="F213" s="34"/>
@@ -15055,7 +15055,7 @@
     <row r="214" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="34"/>
       <c r="B214" s="34"/>
-      <c r="C214" s="76"/>
+      <c r="C214" s="61"/>
       <c r="D214" s="50"/>
       <c r="E214" s="51"/>
       <c r="F214" s="34"/>
@@ -15089,7 +15089,7 @@
     <row r="215" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="34"/>
       <c r="B215" s="34"/>
-      <c r="C215" s="76"/>
+      <c r="C215" s="61"/>
       <c r="D215" s="50"/>
       <c r="E215" s="51"/>
       <c r="F215" s="34"/>
@@ -15123,7 +15123,7 @@
     <row r="216" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="34"/>
       <c r="B216" s="34"/>
-      <c r="C216" s="76"/>
+      <c r="C216" s="61"/>
       <c r="D216" s="50"/>
       <c r="E216" s="51"/>
       <c r="F216" s="34"/>
@@ -15157,7 +15157,7 @@
     <row r="217" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="34"/>
       <c r="B217" s="34"/>
-      <c r="C217" s="76"/>
+      <c r="C217" s="61"/>
       <c r="D217" s="50"/>
       <c r="E217" s="51"/>
       <c r="F217" s="34"/>
@@ -15191,7 +15191,7 @@
     <row r="218" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="34"/>
       <c r="B218" s="34"/>
-      <c r="C218" s="76"/>
+      <c r="C218" s="61"/>
       <c r="D218" s="50"/>
       <c r="E218" s="51"/>
       <c r="F218" s="34"/>
@@ -15225,7 +15225,7 @@
     <row r="219" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="34"/>
       <c r="B219" s="34"/>
-      <c r="C219" s="76"/>
+      <c r="C219" s="61"/>
       <c r="D219" s="50"/>
       <c r="E219" s="51"/>
       <c r="F219" s="34"/>
@@ -15259,7 +15259,7 @@
     <row r="220" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="34"/>
       <c r="B220" s="34"/>
-      <c r="C220" s="76"/>
+      <c r="C220" s="61"/>
       <c r="D220" s="50"/>
       <c r="E220" s="51"/>
       <c r="F220" s="34"/>
@@ -15293,7 +15293,7 @@
     <row r="221" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="34"/>
       <c r="B221" s="34"/>
-      <c r="C221" s="76"/>
+      <c r="C221" s="61"/>
       <c r="D221" s="50"/>
       <c r="E221" s="51"/>
       <c r="F221" s="34"/>
@@ -15327,7 +15327,7 @@
     <row r="222" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="34"/>
       <c r="B222" s="34"/>
-      <c r="C222" s="76"/>
+      <c r="C222" s="61"/>
       <c r="D222" s="50"/>
       <c r="E222" s="51"/>
       <c r="F222" s="34"/>
@@ -15361,7 +15361,7 @@
     <row r="223" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="34"/>
       <c r="B223" s="34"/>
-      <c r="C223" s="76"/>
+      <c r="C223" s="61"/>
       <c r="D223" s="50"/>
       <c r="E223" s="51"/>
       <c r="F223" s="34"/>
@@ -15395,7 +15395,7 @@
     <row r="224" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="34"/>
       <c r="B224" s="34"/>
-      <c r="C224" s="76"/>
+      <c r="C224" s="61"/>
       <c r="D224" s="50"/>
       <c r="E224" s="51"/>
       <c r="F224" s="34"/>
@@ -15429,7 +15429,7 @@
     <row r="225" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="34"/>
       <c r="B225" s="34"/>
-      <c r="C225" s="76"/>
+      <c r="C225" s="61"/>
       <c r="D225" s="50"/>
       <c r="E225" s="51"/>
       <c r="F225" s="34"/>
@@ -15463,7 +15463,7 @@
     <row r="226" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="34"/>
       <c r="B226" s="34"/>
-      <c r="C226" s="76"/>
+      <c r="C226" s="61"/>
       <c r="D226" s="50"/>
       <c r="E226" s="51"/>
       <c r="F226" s="34"/>
@@ -15497,7 +15497,7 @@
     <row r="227" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="34"/>
       <c r="B227" s="34"/>
-      <c r="C227" s="76"/>
+      <c r="C227" s="61"/>
       <c r="D227" s="50"/>
       <c r="E227" s="51"/>
       <c r="F227" s="34"/>
@@ -15531,7 +15531,7 @@
     <row r="228" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="34"/>
       <c r="B228" s="34"/>
-      <c r="C228" s="76"/>
+      <c r="C228" s="61"/>
       <c r="D228" s="50"/>
       <c r="E228" s="51"/>
       <c r="F228" s="34"/>
@@ -15565,7 +15565,7 @@
     <row r="229" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="34"/>
       <c r="B229" s="34"/>
-      <c r="C229" s="76"/>
+      <c r="C229" s="61"/>
       <c r="D229" s="50"/>
       <c r="E229" s="51"/>
       <c r="F229" s="34"/>
@@ -15599,7 +15599,7 @@
     <row r="230" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="34"/>
       <c r="B230" s="34"/>
-      <c r="C230" s="76"/>
+      <c r="C230" s="61"/>
       <c r="D230" s="50"/>
       <c r="E230" s="51"/>
       <c r="F230" s="34"/>
@@ -15633,7 +15633,7 @@
     <row r="231" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="34"/>
       <c r="B231" s="34"/>
-      <c r="C231" s="76"/>
+      <c r="C231" s="61"/>
       <c r="D231" s="50"/>
       <c r="E231" s="51"/>
       <c r="F231" s="34"/>
@@ -17522,64 +17522,150 @@
   </sheetData>
   <autoFilter ref="A9:H24" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="226">
-    <mergeCell ref="C196:E196"/>
-    <mergeCell ref="C197:E197"/>
-    <mergeCell ref="C198:E198"/>
-    <mergeCell ref="C199:E199"/>
-    <mergeCell ref="C200:E200"/>
-    <mergeCell ref="C201:E201"/>
-    <mergeCell ref="C202:E202"/>
-    <mergeCell ref="C187:E187"/>
-    <mergeCell ref="C188:E188"/>
-    <mergeCell ref="C189:E189"/>
-    <mergeCell ref="C190:E190"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="C192:E192"/>
-    <mergeCell ref="C193:E193"/>
-    <mergeCell ref="C194:E194"/>
-    <mergeCell ref="C195:E195"/>
-    <mergeCell ref="C178:E178"/>
-    <mergeCell ref="C179:E179"/>
-    <mergeCell ref="C180:E180"/>
-    <mergeCell ref="C181:E181"/>
-    <mergeCell ref="C182:E182"/>
-    <mergeCell ref="C183:E183"/>
-    <mergeCell ref="C184:E184"/>
-    <mergeCell ref="C185:E185"/>
-    <mergeCell ref="C186:E186"/>
-    <mergeCell ref="C169:E169"/>
-    <mergeCell ref="C170:E170"/>
-    <mergeCell ref="C171:E171"/>
-    <mergeCell ref="C172:E172"/>
-    <mergeCell ref="C173:E173"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C175:E175"/>
-    <mergeCell ref="C176:E176"/>
-    <mergeCell ref="C177:E177"/>
-    <mergeCell ref="C224:E224"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C226:E226"/>
-    <mergeCell ref="C227:E227"/>
-    <mergeCell ref="C228:E228"/>
-    <mergeCell ref="C229:E229"/>
-    <mergeCell ref="C230:E230"/>
-    <mergeCell ref="C231:E231"/>
-    <mergeCell ref="C217:E217"/>
-    <mergeCell ref="C218:E218"/>
-    <mergeCell ref="C219:E219"/>
-    <mergeCell ref="C220:E220"/>
-    <mergeCell ref="C221:E221"/>
-    <mergeCell ref="C222:E222"/>
-    <mergeCell ref="C223:E223"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="C215:E215"/>
-    <mergeCell ref="C216:E216"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="I8:AF9"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C77:E77"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="C81:E81"/>
+    <mergeCell ref="C82:E82"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="C84:E84"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="C86:E86"/>
+    <mergeCell ref="C87:E87"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C90:E90"/>
+    <mergeCell ref="C91:E91"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="C93:E93"/>
+    <mergeCell ref="C94:E94"/>
+    <mergeCell ref="C95:E95"/>
+    <mergeCell ref="C96:E96"/>
+    <mergeCell ref="C97:E97"/>
+    <mergeCell ref="C98:E98"/>
+    <mergeCell ref="C99:E99"/>
+    <mergeCell ref="C100:E100"/>
+    <mergeCell ref="C101:E101"/>
+    <mergeCell ref="C102:E102"/>
+    <mergeCell ref="C103:E103"/>
+    <mergeCell ref="C104:E104"/>
+    <mergeCell ref="C105:E105"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C107:E107"/>
+    <mergeCell ref="C108:E108"/>
+    <mergeCell ref="C109:E109"/>
+    <mergeCell ref="C110:E110"/>
+    <mergeCell ref="C111:E111"/>
+    <mergeCell ref="C112:E112"/>
+    <mergeCell ref="C113:E113"/>
+    <mergeCell ref="C114:E114"/>
+    <mergeCell ref="C115:E115"/>
+    <mergeCell ref="C116:E116"/>
+    <mergeCell ref="C117:E117"/>
+    <mergeCell ref="C118:E118"/>
+    <mergeCell ref="C119:E119"/>
+    <mergeCell ref="C120:E120"/>
+    <mergeCell ref="C121:E121"/>
+    <mergeCell ref="C122:E122"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C124:E124"/>
+    <mergeCell ref="C125:E125"/>
+    <mergeCell ref="C126:E126"/>
+    <mergeCell ref="C127:E127"/>
+    <mergeCell ref="C128:E128"/>
+    <mergeCell ref="C129:E129"/>
+    <mergeCell ref="C130:E130"/>
+    <mergeCell ref="C131:E131"/>
+    <mergeCell ref="C132:E132"/>
+    <mergeCell ref="C133:E133"/>
+    <mergeCell ref="C134:E134"/>
+    <mergeCell ref="C135:E135"/>
+    <mergeCell ref="C136:E136"/>
+    <mergeCell ref="C137:E137"/>
+    <mergeCell ref="C138:E138"/>
+    <mergeCell ref="C139:E139"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C141:E141"/>
+    <mergeCell ref="C142:E142"/>
+    <mergeCell ref="C143:E143"/>
+    <mergeCell ref="C144:E144"/>
+    <mergeCell ref="C145:E145"/>
+    <mergeCell ref="C146:E146"/>
+    <mergeCell ref="C147:E147"/>
+    <mergeCell ref="C148:E148"/>
+    <mergeCell ref="C149:E149"/>
     <mergeCell ref="C150:E150"/>
     <mergeCell ref="C151:E151"/>
     <mergeCell ref="C152:E152"/>
@@ -17604,150 +17690,64 @@
     <mergeCell ref="C166:E166"/>
     <mergeCell ref="C167:E167"/>
     <mergeCell ref="C168:E168"/>
-    <mergeCell ref="C141:E141"/>
-    <mergeCell ref="C142:E142"/>
-    <mergeCell ref="C143:E143"/>
-    <mergeCell ref="C144:E144"/>
-    <mergeCell ref="C145:E145"/>
-    <mergeCell ref="C146:E146"/>
-    <mergeCell ref="C147:E147"/>
-    <mergeCell ref="C148:E148"/>
-    <mergeCell ref="C149:E149"/>
-    <mergeCell ref="C132:E132"/>
-    <mergeCell ref="C133:E133"/>
-    <mergeCell ref="C134:E134"/>
-    <mergeCell ref="C135:E135"/>
-    <mergeCell ref="C136:E136"/>
-    <mergeCell ref="C137:E137"/>
-    <mergeCell ref="C138:E138"/>
-    <mergeCell ref="C139:E139"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C124:E124"/>
-    <mergeCell ref="C125:E125"/>
-    <mergeCell ref="C126:E126"/>
-    <mergeCell ref="C127:E127"/>
-    <mergeCell ref="C128:E128"/>
-    <mergeCell ref="C129:E129"/>
-    <mergeCell ref="C130:E130"/>
-    <mergeCell ref="C131:E131"/>
-    <mergeCell ref="C114:E114"/>
-    <mergeCell ref="C115:E115"/>
-    <mergeCell ref="C116:E116"/>
-    <mergeCell ref="C117:E117"/>
-    <mergeCell ref="C118:E118"/>
-    <mergeCell ref="C119:E119"/>
-    <mergeCell ref="C120:E120"/>
-    <mergeCell ref="C121:E121"/>
-    <mergeCell ref="C122:E122"/>
-    <mergeCell ref="C105:E105"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C107:E107"/>
-    <mergeCell ref="C108:E108"/>
-    <mergeCell ref="C109:E109"/>
-    <mergeCell ref="C110:E110"/>
-    <mergeCell ref="C111:E111"/>
-    <mergeCell ref="C112:E112"/>
-    <mergeCell ref="C113:E113"/>
-    <mergeCell ref="C96:E96"/>
-    <mergeCell ref="C97:E97"/>
-    <mergeCell ref="C98:E98"/>
-    <mergeCell ref="C99:E99"/>
-    <mergeCell ref="C100:E100"/>
-    <mergeCell ref="C101:E101"/>
-    <mergeCell ref="C102:E102"/>
-    <mergeCell ref="C103:E103"/>
-    <mergeCell ref="C104:E104"/>
-    <mergeCell ref="C87:E87"/>
-    <mergeCell ref="C88:E88"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C90:E90"/>
-    <mergeCell ref="C91:E91"/>
-    <mergeCell ref="C92:E92"/>
-    <mergeCell ref="C93:E93"/>
-    <mergeCell ref="C94:E94"/>
-    <mergeCell ref="C95:E95"/>
-    <mergeCell ref="C78:E78"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="C81:E81"/>
-    <mergeCell ref="C82:E82"/>
-    <mergeCell ref="C83:E83"/>
-    <mergeCell ref="C84:E84"/>
-    <mergeCell ref="C85:E85"/>
-    <mergeCell ref="C86:E86"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="C77:E77"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="I8:AF9"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="C215:E215"/>
+    <mergeCell ref="C216:E216"/>
+    <mergeCell ref="C224:E224"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C226:E226"/>
+    <mergeCell ref="C227:E227"/>
+    <mergeCell ref="C228:E228"/>
+    <mergeCell ref="C229:E229"/>
+    <mergeCell ref="C230:E230"/>
+    <mergeCell ref="C231:E231"/>
+    <mergeCell ref="C217:E217"/>
+    <mergeCell ref="C218:E218"/>
+    <mergeCell ref="C219:E219"/>
+    <mergeCell ref="C220:E220"/>
+    <mergeCell ref="C221:E221"/>
+    <mergeCell ref="C222:E222"/>
+    <mergeCell ref="C223:E223"/>
+    <mergeCell ref="C169:E169"/>
+    <mergeCell ref="C170:E170"/>
+    <mergeCell ref="C171:E171"/>
+    <mergeCell ref="C172:E172"/>
+    <mergeCell ref="C173:E173"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C175:E175"/>
+    <mergeCell ref="C176:E176"/>
+    <mergeCell ref="C177:E177"/>
+    <mergeCell ref="C178:E178"/>
+    <mergeCell ref="C179:E179"/>
+    <mergeCell ref="C180:E180"/>
+    <mergeCell ref="C181:E181"/>
+    <mergeCell ref="C182:E182"/>
+    <mergeCell ref="C183:E183"/>
+    <mergeCell ref="C184:E184"/>
+    <mergeCell ref="C185:E185"/>
+    <mergeCell ref="C186:E186"/>
+    <mergeCell ref="C196:E196"/>
+    <mergeCell ref="C197:E197"/>
+    <mergeCell ref="C198:E198"/>
+    <mergeCell ref="C199:E199"/>
+    <mergeCell ref="C200:E200"/>
+    <mergeCell ref="C201:E201"/>
+    <mergeCell ref="C202:E202"/>
+    <mergeCell ref="C187:E187"/>
+    <mergeCell ref="C188:E188"/>
+    <mergeCell ref="C189:E189"/>
+    <mergeCell ref="C190:E190"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C192:E192"/>
+    <mergeCell ref="C193:E193"/>
+    <mergeCell ref="C194:E194"/>
+    <mergeCell ref="C195:E195"/>
   </mergeCells>
   <conditionalFormatting sqref="G991:G1002">
     <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
@@ -17887,70 +17887,70 @@
       <c r="E1" s="43"/>
     </row>
     <row r="2" spans="2:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="79"/>
-      <c r="R2" s="77" t="s">
+      <c r="B2" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="82"/>
+      <c r="R2" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="80"/>
-      <c r="T2" s="81" t="s">
+      <c r="S2" s="83"/>
+      <c r="T2" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="U2" s="80"/>
-      <c r="V2" s="82" t="s">
+      <c r="U2" s="83"/>
+      <c r="V2" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="W2" s="79"/>
+      <c r="W2" s="82"/>
     </row>
     <row r="3" spans="2:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="83" t="str">
+      <c r="B3" s="86" t="str">
         <f>Config!A6</f>
         <v>Modulo Almacenes del Sistema de Información XXXX</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="79"/>
-      <c r="R3" s="83">
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="82"/>
+      <c r="R3" s="86">
         <f>Config!A9</f>
         <v>1</v>
       </c>
-      <c r="S3" s="79"/>
-      <c r="T3" s="84">
+      <c r="S3" s="82"/>
+      <c r="T3" s="87">
         <f>Config!B9</f>
         <v>44874</v>
       </c>
-      <c r="U3" s="79"/>
-      <c r="V3" s="85">
+      <c r="U3" s="82"/>
+      <c r="V3" s="88">
         <f>Config!C9</f>
         <v>15</v>
       </c>
-      <c r="W3" s="79"/>
+      <c r="W3" s="82"/>
     </row>
     <row r="4" spans="2:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="24"/>
@@ -18123,15 +18123,15 @@
       </c>
       <c r="C58" s="47">
         <f>SUMIF(Datos!$H$11:$H$992,$A58,Datos!J$11:J$1003)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D58" s="47">
         <f>SUMIF(Datos!$H$11:$H$992,$A58,Datos!K$11:K$1003)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E58" s="47">
         <f>SUMIF(Datos!$H$11:$H$992,$A58,Datos!L$11:L$1003)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F58" s="47">
         <f>SUMIF(Datos!$H$11:$H$992,$A58,Datos!M$11:M$1003)</f>
@@ -18335,7 +18335,7 @@
       </c>
       <c r="E60" s="47">
         <f>SUMIF(Datos!$H$11:$H$992,$A60,Datos!L$11:L$1003)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F60" s="47">
         <f>SUMIF(Datos!$H$11:$H$992,$A60,Datos!M$11:M$1003)</f>

</xml_diff>